<commit_message>
Documentos Anexos para el analisis
</commit_message>
<xml_diff>
--- a/Planteamiento de Base de DATOS.xlsx
+++ b/Planteamiento de Base de DATOS.xlsx
@@ -1094,7 +1094,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="12">
+  <borders count="11">
     <border>
       <left/>
       <right/>
@@ -1176,15 +1176,6 @@
       <bottom style="thin">
         <color indexed="64"/>
       </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top/>
-      <bottom/>
       <diagonal/>
     </border>
     <border>
@@ -1349,6 +1340,56 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="49" fontId="7" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="7" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="164" fontId="7" fillId="11" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="49" fontId="7" fillId="11" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="7" fillId="11" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1361,6 +1402,9 @@
     <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1370,75 +1414,16 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="49" fontId="7" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="164" fontId="7" fillId="11" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="49" fontId="7" fillId="11" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="7" fillId="11" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1450,6 +1435,15 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -1459,14 +1453,11 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1761,8 +1752,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:AX74"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="AI19" sqref="AI19"/>
+    <sheetView tabSelected="1" topLeftCell="M40" workbookViewId="0">
+      <selection activeCell="AB8" sqref="AB8:AI8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1809,50 +1800,50 @@
       <c r="AS1" s="50"/>
     </row>
     <row r="2" spans="2:50" ht="25.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="C2" s="60" t="s">
+      <c r="C2" s="87" t="s">
         <v>0</v>
       </c>
-      <c r="D2" s="60"/>
-      <c r="E2" s="60"/>
-      <c r="F2" s="60"/>
+      <c r="D2" s="87"/>
+      <c r="E2" s="87"/>
+      <c r="F2" s="87"/>
       <c r="G2" s="47"/>
       <c r="H2" s="47"/>
-      <c r="M2" s="56" t="s">
+      <c r="M2" s="82" t="s">
         <v>33</v>
       </c>
-      <c r="N2" s="57"/>
-      <c r="O2" s="57"/>
-      <c r="P2" s="57"/>
-      <c r="Q2" s="58"/>
-      <c r="S2" s="61" t="s">
+      <c r="N2" s="83"/>
+      <c r="O2" s="83"/>
+      <c r="P2" s="83"/>
+      <c r="Q2" s="84"/>
+      <c r="S2" s="88" t="s">
         <v>46</v>
       </c>
-      <c r="T2" s="62"/>
-      <c r="V2" s="60" t="s">
+      <c r="T2" s="89"/>
+      <c r="V2" s="87" t="s">
         <v>291</v>
       </c>
-      <c r="W2" s="60"/>
-      <c r="AA2" s="56" t="s">
+      <c r="W2" s="87"/>
+      <c r="AA2" s="82" t="s">
         <v>51</v>
       </c>
-      <c r="AB2" s="57"/>
-      <c r="AC2" s="57"/>
-      <c r="AD2" s="57"/>
-      <c r="AE2" s="57"/>
-      <c r="AF2" s="57"/>
-      <c r="AG2" s="57"/>
-      <c r="AH2" s="57"/>
-      <c r="AI2" s="57"/>
-      <c r="AJ2" s="58"/>
-      <c r="AN2" s="74"/>
-      <c r="AO2" s="74"/>
-      <c r="AP2" s="71"/>
-      <c r="AQ2" s="71"/>
-      <c r="AR2" s="71"/>
-      <c r="AS2" s="71"/>
-      <c r="AT2" s="71"/>
-      <c r="AU2" s="71"/>
-      <c r="AV2" s="71"/>
+      <c r="AB2" s="83"/>
+      <c r="AC2" s="83"/>
+      <c r="AD2" s="83"/>
+      <c r="AE2" s="83"/>
+      <c r="AF2" s="83"/>
+      <c r="AG2" s="83"/>
+      <c r="AH2" s="83"/>
+      <c r="AI2" s="83"/>
+      <c r="AJ2" s="84"/>
+      <c r="AN2" s="86"/>
+      <c r="AO2" s="86"/>
+      <c r="AP2" s="63"/>
+      <c r="AQ2" s="63"/>
+      <c r="AR2" s="63"/>
+      <c r="AS2" s="63"/>
+      <c r="AT2" s="63"/>
+      <c r="AU2" s="63"/>
+      <c r="AV2" s="63"/>
     </row>
     <row r="3" spans="2:50" x14ac:dyDescent="0.25">
       <c r="C3" s="6" t="s">
@@ -1899,21 +1890,21 @@
       <c r="AA3" s="46" t="s">
         <v>59</v>
       </c>
-      <c r="AB3" s="102" t="s">
+      <c r="AB3" s="97" t="s">
         <v>60</v>
       </c>
-      <c r="AC3" s="103"/>
-      <c r="AD3" s="103"/>
-      <c r="AE3" s="103"/>
-      <c r="AF3" s="103"/>
-      <c r="AG3" s="103"/>
-      <c r="AH3" s="103"/>
-      <c r="AI3" s="104"/>
+      <c r="AC3" s="98"/>
+      <c r="AD3" s="98"/>
+      <c r="AE3" s="98"/>
+      <c r="AF3" s="98"/>
+      <c r="AG3" s="98"/>
+      <c r="AH3" s="98"/>
+      <c r="AI3" s="99"/>
       <c r="AJ3" s="6" t="s">
         <v>177</v>
       </c>
-      <c r="AN3" s="75"/>
-      <c r="AO3" s="76"/>
+      <c r="AN3" s="66"/>
+      <c r="AO3" s="67"/>
       <c r="AT3" s="7"/>
       <c r="AU3" s="7"/>
       <c r="AV3" s="7"/>
@@ -1968,21 +1959,21 @@
       <c r="AA4" s="45" t="s">
         <v>298</v>
       </c>
-      <c r="AB4" s="96" t="s">
+      <c r="AB4" s="94" t="s">
         <v>52</v>
       </c>
-      <c r="AC4" s="97"/>
-      <c r="AD4" s="97"/>
-      <c r="AE4" s="97"/>
-      <c r="AF4" s="97"/>
-      <c r="AG4" s="97"/>
-      <c r="AH4" s="97"/>
-      <c r="AI4" s="98"/>
+      <c r="AC4" s="95"/>
+      <c r="AD4" s="95"/>
+      <c r="AE4" s="95"/>
+      <c r="AF4" s="95"/>
+      <c r="AG4" s="95"/>
+      <c r="AH4" s="95"/>
+      <c r="AI4" s="96"/>
       <c r="AJ4" s="3">
         <v>0</v>
       </c>
-      <c r="AN4" s="75"/>
-      <c r="AO4" s="76"/>
+      <c r="AN4" s="66"/>
+      <c r="AO4" s="67"/>
     </row>
     <row r="5" spans="2:50" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C5" s="1" t="s">
@@ -2032,21 +2023,21 @@
       <c r="AA5" s="45" t="s">
         <v>299</v>
       </c>
-      <c r="AB5" s="96" t="s">
+      <c r="AB5" s="94" t="s">
         <v>53</v>
       </c>
-      <c r="AC5" s="97"/>
-      <c r="AD5" s="97"/>
-      <c r="AE5" s="97"/>
-      <c r="AF5" s="97"/>
-      <c r="AG5" s="97"/>
-      <c r="AH5" s="97"/>
-      <c r="AI5" s="98"/>
+      <c r="AC5" s="95"/>
+      <c r="AD5" s="95"/>
+      <c r="AE5" s="95"/>
+      <c r="AF5" s="95"/>
+      <c r="AG5" s="95"/>
+      <c r="AH5" s="95"/>
+      <c r="AI5" s="96"/>
       <c r="AJ5" s="3">
         <v>0</v>
       </c>
-      <c r="AN5" s="81"/>
-      <c r="AO5" s="82"/>
+      <c r="AN5" s="72"/>
+      <c r="AO5" s="73"/>
     </row>
     <row r="6" spans="2:50" ht="15.75" x14ac:dyDescent="0.25">
       <c r="C6" s="1" t="s">
@@ -2096,21 +2087,21 @@
       <c r="AA6" s="45" t="s">
         <v>300</v>
       </c>
-      <c r="AB6" s="96" t="s">
+      <c r="AB6" s="94" t="s">
         <v>54</v>
       </c>
-      <c r="AC6" s="97"/>
-      <c r="AD6" s="97"/>
-      <c r="AE6" s="97"/>
-      <c r="AF6" s="97"/>
-      <c r="AG6" s="97"/>
-      <c r="AH6" s="97"/>
-      <c r="AI6" s="98"/>
+      <c r="AC6" s="95"/>
+      <c r="AD6" s="95"/>
+      <c r="AE6" s="95"/>
+      <c r="AF6" s="95"/>
+      <c r="AG6" s="95"/>
+      <c r="AH6" s="95"/>
+      <c r="AI6" s="96"/>
       <c r="AJ6" s="3">
         <v>0</v>
       </c>
-      <c r="AN6" s="81"/>
-      <c r="AO6" s="82"/>
+      <c r="AN6" s="72"/>
+      <c r="AO6" s="73"/>
     </row>
     <row r="7" spans="2:50" ht="15.75" x14ac:dyDescent="0.25">
       <c r="C7" s="1" t="s">
@@ -2160,16 +2151,16 @@
       <c r="AA7" s="45" t="s">
         <v>301</v>
       </c>
-      <c r="AB7" s="96" t="s">
+      <c r="AB7" s="94" t="s">
         <v>55</v>
       </c>
-      <c r="AC7" s="97"/>
-      <c r="AD7" s="97"/>
-      <c r="AE7" s="97"/>
-      <c r="AF7" s="97"/>
-      <c r="AG7" s="97"/>
-      <c r="AH7" s="97"/>
-      <c r="AI7" s="98"/>
+      <c r="AC7" s="95"/>
+      <c r="AD7" s="95"/>
+      <c r="AE7" s="95"/>
+      <c r="AF7" s="95"/>
+      <c r="AG7" s="95"/>
+      <c r="AH7" s="95"/>
+      <c r="AI7" s="96"/>
       <c r="AJ7" s="3">
         <v>0</v>
       </c>
@@ -2216,16 +2207,16 @@
       <c r="AA8" s="45" t="s">
         <v>302</v>
       </c>
-      <c r="AB8" s="96" t="s">
+      <c r="AB8" s="94" t="s">
         <v>56</v>
       </c>
-      <c r="AC8" s="97"/>
-      <c r="AD8" s="97"/>
-      <c r="AE8" s="97"/>
-      <c r="AF8" s="97"/>
-      <c r="AG8" s="97"/>
-      <c r="AH8" s="97"/>
-      <c r="AI8" s="98"/>
+      <c r="AC8" s="95"/>
+      <c r="AD8" s="95"/>
+      <c r="AE8" s="95"/>
+      <c r="AF8" s="95"/>
+      <c r="AG8" s="95"/>
+      <c r="AH8" s="95"/>
+      <c r="AI8" s="96"/>
       <c r="AJ8" s="3">
         <v>0</v>
       </c>
@@ -2252,16 +2243,16 @@
       <c r="AA9" s="45" t="s">
         <v>303</v>
       </c>
-      <c r="AB9" s="99" t="s">
+      <c r="AB9" s="100" t="s">
         <v>57</v>
       </c>
-      <c r="AC9" s="100"/>
-      <c r="AD9" s="100"/>
-      <c r="AE9" s="100"/>
-      <c r="AF9" s="100"/>
-      <c r="AG9" s="100"/>
-      <c r="AH9" s="100"/>
-      <c r="AI9" s="101"/>
+      <c r="AC9" s="101"/>
+      <c r="AD9" s="101"/>
+      <c r="AE9" s="101"/>
+      <c r="AF9" s="101"/>
+      <c r="AG9" s="101"/>
+      <c r="AH9" s="101"/>
+      <c r="AI9" s="102"/>
       <c r="AJ9" s="3">
         <v>0</v>
       </c>
@@ -2288,16 +2279,16 @@
       <c r="AA10" s="45" t="s">
         <v>304</v>
       </c>
-      <c r="AB10" s="99" t="s">
+      <c r="AB10" s="100" t="s">
         <v>58</v>
       </c>
-      <c r="AC10" s="100"/>
-      <c r="AD10" s="100"/>
-      <c r="AE10" s="100"/>
-      <c r="AF10" s="100"/>
-      <c r="AG10" s="100"/>
-      <c r="AH10" s="100"/>
-      <c r="AI10" s="101"/>
+      <c r="AC10" s="101"/>
+      <c r="AD10" s="101"/>
+      <c r="AE10" s="101"/>
+      <c r="AF10" s="101"/>
+      <c r="AG10" s="101"/>
+      <c r="AH10" s="101"/>
+      <c r="AI10" s="102"/>
       <c r="AJ10" s="3">
         <v>0</v>
       </c>
@@ -2321,16 +2312,16 @@
       <c r="AA11" s="45" t="s">
         <v>305</v>
       </c>
-      <c r="AB11" s="96" t="s">
+      <c r="AB11" s="94" t="s">
         <v>171</v>
       </c>
-      <c r="AC11" s="97"/>
-      <c r="AD11" s="97"/>
-      <c r="AE11" s="97"/>
-      <c r="AF11" s="97"/>
-      <c r="AG11" s="97"/>
-      <c r="AH11" s="97"/>
-      <c r="AI11" s="98"/>
+      <c r="AC11" s="95"/>
+      <c r="AD11" s="95"/>
+      <c r="AE11" s="95"/>
+      <c r="AF11" s="95"/>
+      <c r="AG11" s="95"/>
+      <c r="AH11" s="95"/>
+      <c r="AI11" s="96"/>
       <c r="AJ11" s="3">
         <v>18000</v>
       </c>
@@ -2344,87 +2335,87 @@
       <c r="AA12" s="45" t="s">
         <v>306</v>
       </c>
-      <c r="AB12" s="96" t="s">
+      <c r="AB12" s="94" t="s">
         <v>179</v>
       </c>
-      <c r="AC12" s="97"/>
-      <c r="AD12" s="97"/>
-      <c r="AE12" s="97"/>
-      <c r="AF12" s="97"/>
-      <c r="AG12" s="97"/>
-      <c r="AH12" s="97"/>
-      <c r="AI12" s="98"/>
+      <c r="AC12" s="95"/>
+      <c r="AD12" s="95"/>
+      <c r="AE12" s="95"/>
+      <c r="AF12" s="95"/>
+      <c r="AG12" s="95"/>
+      <c r="AH12" s="95"/>
+      <c r="AI12" s="96"/>
       <c r="AJ12" s="1" t="s">
         <v>180</v>
       </c>
-      <c r="AN12" s="65"/>
-      <c r="AO12" s="63"/>
+      <c r="AN12" s="58"/>
+      <c r="AO12" s="56"/>
       <c r="AP12" s="7"/>
       <c r="AQ12" s="41"/>
     </row>
     <row r="13" spans="2:50" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="AN13" s="65"/>
-      <c r="AO13" s="63"/>
+      <c r="AN13" s="58"/>
+      <c r="AO13" s="56"/>
       <c r="AP13" s="7"/>
       <c r="AQ13" s="41"/>
     </row>
     <row r="14" spans="2:50" ht="20.25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="C14" s="69"/>
-      <c r="D14" s="69"/>
-      <c r="E14" s="69"/>
-      <c r="F14" s="69"/>
-      <c r="G14" s="69"/>
-      <c r="H14" s="69"/>
-      <c r="M14" s="83" t="s">
+      <c r="C14" s="90"/>
+      <c r="D14" s="90"/>
+      <c r="E14" s="90"/>
+      <c r="F14" s="90"/>
+      <c r="G14" s="90"/>
+      <c r="H14" s="90"/>
+      <c r="M14" s="103" t="s">
         <v>183</v>
       </c>
-      <c r="N14" s="84"/>
-      <c r="O14" s="84"/>
-      <c r="P14" s="84"/>
-      <c r="Q14" s="84"/>
-      <c r="R14" s="84"/>
-      <c r="S14" s="84"/>
-      <c r="T14" s="84"/>
-      <c r="U14" s="84"/>
-      <c r="V14" s="84"/>
-      <c r="W14" s="84"/>
-      <c r="X14" s="84"/>
-      <c r="Y14" s="84"/>
-      <c r="AA14" s="56" t="s">
+      <c r="N14" s="103"/>
+      <c r="O14" s="103"/>
+      <c r="P14" s="103"/>
+      <c r="Q14" s="103"/>
+      <c r="R14" s="103"/>
+      <c r="S14" s="103"/>
+      <c r="T14" s="103"/>
+      <c r="U14" s="103"/>
+      <c r="V14" s="103"/>
+      <c r="W14" s="103"/>
+      <c r="X14" s="103"/>
+      <c r="Y14" s="103"/>
+      <c r="AA14" s="82" t="s">
         <v>193</v>
       </c>
-      <c r="AB14" s="57"/>
-      <c r="AC14" s="57"/>
-      <c r="AD14" s="57"/>
-      <c r="AE14" s="57"/>
-      <c r="AF14" s="57"/>
-      <c r="AG14" s="57"/>
-      <c r="AH14" s="58"/>
-      <c r="AI14" s="71"/>
-      <c r="AJ14" s="59" t="s">
+      <c r="AB14" s="83"/>
+      <c r="AC14" s="83"/>
+      <c r="AD14" s="83"/>
+      <c r="AE14" s="83"/>
+      <c r="AF14" s="83"/>
+      <c r="AG14" s="83"/>
+      <c r="AH14" s="84"/>
+      <c r="AI14" s="63"/>
+      <c r="AJ14" s="85" t="s">
         <v>194</v>
       </c>
-      <c r="AK14" s="59"/>
-      <c r="AL14" s="59"/>
-      <c r="AM14" s="59"/>
-      <c r="AN14" s="59"/>
-      <c r="AO14" s="59"/>
-      <c r="AP14" s="59"/>
+      <c r="AK14" s="85"/>
+      <c r="AL14" s="85"/>
+      <c r="AM14" s="85"/>
+      <c r="AN14" s="85"/>
+      <c r="AO14" s="85"/>
+      <c r="AP14" s="85"/>
     </row>
     <row r="15" spans="2:50" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="B15" s="59" t="s">
+      <c r="B15" s="85" t="s">
         <v>184</v>
       </c>
-      <c r="C15" s="59"/>
-      <c r="D15" s="59"/>
-      <c r="E15" s="59"/>
-      <c r="F15" s="59"/>
-      <c r="G15" s="59"/>
-      <c r="H15" s="59"/>
-      <c r="I15" s="59"/>
-      <c r="J15" s="59"/>
-      <c r="K15" s="59"/>
-      <c r="L15" s="71"/>
+      <c r="C15" s="85"/>
+      <c r="D15" s="85"/>
+      <c r="E15" s="85"/>
+      <c r="F15" s="85"/>
+      <c r="G15" s="85"/>
+      <c r="H15" s="85"/>
+      <c r="I15" s="85"/>
+      <c r="J15" s="85"/>
+      <c r="K15" s="85"/>
+      <c r="L15" s="63"/>
       <c r="M15" s="39" t="s">
         <v>176</v>
       </c>
@@ -2434,11 +2425,11 @@
       <c r="O15" s="38" t="s">
         <v>46</v>
       </c>
-      <c r="P15" s="89" t="s">
+      <c r="P15" s="91" t="s">
         <v>60</v>
       </c>
-      <c r="Q15" s="90"/>
-      <c r="R15" s="91"/>
+      <c r="Q15" s="92"/>
+      <c r="R15" s="93"/>
       <c r="S15" s="40" t="s">
         <v>69</v>
       </c>
@@ -2457,16 +2448,16 @@
       <c r="X15" s="12" t="s">
         <v>291</v>
       </c>
-      <c r="Y15" s="6" t="s">
+      <c r="Y15" s="40" t="s">
         <v>307</v>
       </c>
       <c r="AA15" s="3" t="s">
         <v>196</v>
       </c>
-      <c r="AB15" s="77" t="s">
+      <c r="AB15" s="68" t="s">
         <v>292</v>
       </c>
-      <c r="AC15" s="78" t="s">
+      <c r="AC15" s="69" t="s">
         <v>154</v>
       </c>
       <c r="AD15" s="3" t="s">
@@ -2475,10 +2466,10 @@
       <c r="AE15" s="3" t="s">
         <v>155</v>
       </c>
-      <c r="AF15" s="77" t="s">
+      <c r="AF15" s="68" t="s">
         <v>310</v>
       </c>
-      <c r="AG15" s="77" t="s">
+      <c r="AG15" s="68" t="s">
         <v>309</v>
       </c>
       <c r="AH15" s="3" t="s">
@@ -2488,10 +2479,10 @@
       <c r="AJ15" s="1" t="s">
         <v>195</v>
       </c>
-      <c r="AK15" s="73" t="s">
+      <c r="AK15" s="65" t="s">
         <v>292</v>
       </c>
-      <c r="AL15" s="68" t="s">
+      <c r="AL15" s="61" t="s">
         <v>154</v>
       </c>
       <c r="AM15" s="1" t="s">
@@ -2500,7 +2491,7 @@
       <c r="AN15" s="1" t="s">
         <v>155</v>
       </c>
-      <c r="AO15" s="73" t="s">
+      <c r="AO15" s="65" t="s">
         <v>214</v>
       </c>
       <c r="AP15" s="1" t="s">
@@ -2533,20 +2524,20 @@
         <v>190</v>
       </c>
       <c r="L16" s="41"/>
-      <c r="M16" s="92" t="s">
+      <c r="M16" s="104" t="s">
         <v>35</v>
       </c>
-      <c r="N16" s="92" t="s">
+      <c r="N16" s="78" t="s">
         <v>13</v>
       </c>
-      <c r="O16" s="92" t="s">
+      <c r="O16" s="78" t="s">
         <v>287</v>
       </c>
-      <c r="P16" s="93" t="s">
+      <c r="P16" s="79" t="s">
         <v>61</v>
       </c>
-      <c r="Q16" s="94"/>
-      <c r="R16" s="95"/>
+      <c r="Q16" s="80"/>
+      <c r="R16" s="81"/>
       <c r="S16" s="35" t="s">
         <v>120</v>
       </c>
@@ -2580,19 +2571,19 @@
       <c r="AD16" s="3" t="s">
         <v>120</v>
       </c>
-      <c r="AE16" s="72" t="s">
-        <v>294</v>
-      </c>
-      <c r="AF16" s="72">
-        <v>1</v>
-      </c>
-      <c r="AG16" s="77" t="s">
+      <c r="AE16" s="64" t="s">
+        <v>294</v>
+      </c>
+      <c r="AF16" s="64">
+        <v>1</v>
+      </c>
+      <c r="AG16" s="68" t="s">
         <v>308</v>
       </c>
       <c r="AH16" s="3">
         <v>70000</v>
       </c>
-      <c r="AI16" s="65"/>
+      <c r="AI16" s="58"/>
       <c r="AJ16" s="1" t="s">
         <v>205</v>
       </c>
@@ -2605,10 +2596,10 @@
       <c r="AM16" s="1" t="s">
         <v>120</v>
       </c>
-      <c r="AN16" s="73" t="s">
-        <v>294</v>
-      </c>
-      <c r="AO16" s="68">
+      <c r="AN16" s="65" t="s">
+        <v>294</v>
+      </c>
+      <c r="AO16" s="61">
         <v>1</v>
       </c>
       <c r="AP16" s="1">
@@ -2616,7 +2607,7 @@
       </c>
     </row>
     <row r="17" spans="2:42" x14ac:dyDescent="0.25">
-      <c r="B17" t="s">
+      <c r="B17" s="1" t="s">
         <v>189</v>
       </c>
       <c r="C17" s="3" t="s">
@@ -2640,17 +2631,17 @@
       <c r="M17" s="34" t="s">
         <v>36</v>
       </c>
-      <c r="N17" s="92" t="s">
+      <c r="N17" s="78" t="s">
         <v>13</v>
       </c>
-      <c r="O17" s="92" t="s">
+      <c r="O17" s="78" t="s">
         <v>287</v>
       </c>
-      <c r="P17" s="93" t="s">
+      <c r="P17" s="79" t="s">
         <v>61</v>
       </c>
-      <c r="Q17" s="94"/>
-      <c r="R17" s="95"/>
+      <c r="Q17" s="80"/>
+      <c r="R17" s="81"/>
       <c r="S17" s="35" t="s">
         <v>121</v>
       </c>
@@ -2684,19 +2675,19 @@
       <c r="AD17" s="3" t="s">
         <v>121</v>
       </c>
-      <c r="AE17" s="72" t="s">
-        <v>294</v>
-      </c>
-      <c r="AF17" s="72">
-        <v>1</v>
-      </c>
-      <c r="AG17" s="77" t="s">
+      <c r="AE17" s="64" t="s">
+        <v>294</v>
+      </c>
+      <c r="AF17" s="64">
+        <v>1</v>
+      </c>
+      <c r="AG17" s="68" t="s">
         <v>308</v>
       </c>
       <c r="AH17" s="3">
         <v>70000</v>
       </c>
-      <c r="AI17" s="65"/>
+      <c r="AI17" s="58"/>
       <c r="AJ17" s="1" t="s">
         <v>207</v>
       </c>
@@ -2709,10 +2700,10 @@
       <c r="AM17" s="1" t="s">
         <v>121</v>
       </c>
-      <c r="AN17" s="73" t="s">
-        <v>294</v>
-      </c>
-      <c r="AO17" s="68">
+      <c r="AN17" s="65" t="s">
+        <v>294</v>
+      </c>
+      <c r="AO17" s="61">
         <v>1</v>
       </c>
       <c r="AP17" s="1">
@@ -2720,31 +2711,31 @@
       </c>
     </row>
     <row r="18" spans="2:42" x14ac:dyDescent="0.25">
-      <c r="B18" t="s">
+      <c r="B18" s="1" t="s">
         <v>284</v>
       </c>
       <c r="C18" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="D18" s="63"/>
-      <c r="E18" s="70"/>
-      <c r="F18" s="70"/>
-      <c r="G18" s="70"/>
-      <c r="H18" s="70"/>
+      <c r="D18" s="56"/>
+      <c r="E18" s="62"/>
+      <c r="F18" s="62"/>
+      <c r="G18" s="62"/>
+      <c r="H18" s="62"/>
       <c r="M18" s="34" t="s">
         <v>37</v>
       </c>
-      <c r="N18" s="92" t="s">
+      <c r="N18" s="78" t="s">
         <v>13</v>
       </c>
-      <c r="O18" s="92" t="s">
+      <c r="O18" s="78" t="s">
         <v>287</v>
       </c>
-      <c r="P18" s="93" t="s">
+      <c r="P18" s="79" t="s">
         <v>61</v>
       </c>
-      <c r="Q18" s="94"/>
-      <c r="R18" s="95"/>
+      <c r="Q18" s="80"/>
+      <c r="R18" s="81"/>
       <c r="S18" s="35" t="s">
         <v>122</v>
       </c>
@@ -2778,13 +2769,13 @@
       <c r="AD18" s="3" t="s">
         <v>122</v>
       </c>
-      <c r="AE18" s="72" t="s">
-        <v>294</v>
-      </c>
-      <c r="AF18" s="72">
-        <v>1</v>
-      </c>
-      <c r="AG18" s="77" t="s">
+      <c r="AE18" s="64" t="s">
+        <v>294</v>
+      </c>
+      <c r="AF18" s="64">
+        <v>1</v>
+      </c>
+      <c r="AG18" s="68" t="s">
         <v>308</v>
       </c>
       <c r="AH18" s="3">
@@ -2803,10 +2794,10 @@
       <c r="AM18" s="1" t="s">
         <v>122</v>
       </c>
-      <c r="AN18" s="73" t="s">
-        <v>294</v>
-      </c>
-      <c r="AO18" s="68">
+      <c r="AN18" s="65" t="s">
+        <v>294</v>
+      </c>
+      <c r="AO18" s="61">
         <v>1</v>
       </c>
       <c r="AP18" s="1">
@@ -2815,25 +2806,25 @@
     </row>
     <row r="19" spans="2:42" x14ac:dyDescent="0.25">
       <c r="C19" s="41"/>
-      <c r="D19" s="63"/>
-      <c r="E19" s="70"/>
-      <c r="F19" s="70"/>
-      <c r="G19" s="70"/>
-      <c r="H19" s="70"/>
+      <c r="D19" s="56"/>
+      <c r="E19" s="62"/>
+      <c r="F19" s="62"/>
+      <c r="G19" s="62"/>
+      <c r="H19" s="62"/>
       <c r="M19" s="34" t="s">
         <v>38</v>
       </c>
-      <c r="N19" s="92" t="s">
+      <c r="N19" s="78" t="s">
         <v>13</v>
       </c>
-      <c r="O19" s="92" t="s">
+      <c r="O19" s="78" t="s">
         <v>287</v>
       </c>
-      <c r="P19" s="93" t="s">
+      <c r="P19" s="79" t="s">
         <v>61</v>
       </c>
-      <c r="Q19" s="94"/>
-      <c r="R19" s="95"/>
+      <c r="Q19" s="80"/>
+      <c r="R19" s="81"/>
       <c r="S19" s="35" t="s">
         <v>123</v>
       </c>
@@ -2867,13 +2858,13 @@
       <c r="AD19" s="3" t="s">
         <v>123</v>
       </c>
-      <c r="AE19" s="72" t="s">
-        <v>294</v>
-      </c>
-      <c r="AF19" s="72">
-        <v>1</v>
-      </c>
-      <c r="AG19" s="77" t="s">
+      <c r="AE19" s="64" t="s">
+        <v>294</v>
+      </c>
+      <c r="AF19" s="64">
+        <v>1</v>
+      </c>
+      <c r="AG19" s="68" t="s">
         <v>308</v>
       </c>
       <c r="AH19" s="3">
@@ -2892,10 +2883,10 @@
       <c r="AM19" s="1" t="s">
         <v>123</v>
       </c>
-      <c r="AN19" s="73" t="s">
-        <v>294</v>
-      </c>
-      <c r="AO19" s="68">
+      <c r="AN19" s="65" t="s">
+        <v>294</v>
+      </c>
+      <c r="AO19" s="61">
         <v>1</v>
       </c>
       <c r="AP19" s="1">
@@ -2904,25 +2895,25 @@
     </row>
     <row r="20" spans="2:42" x14ac:dyDescent="0.25">
       <c r="C20" s="41"/>
-      <c r="D20" s="63"/>
-      <c r="E20" s="70"/>
-      <c r="F20" s="70"/>
-      <c r="G20" s="70"/>
-      <c r="H20" s="70"/>
+      <c r="D20" s="56"/>
+      <c r="E20" s="62"/>
+      <c r="F20" s="62"/>
+      <c r="G20" s="62"/>
+      <c r="H20" s="62"/>
       <c r="M20" s="34" t="s">
         <v>39</v>
       </c>
-      <c r="N20" s="92" t="s">
+      <c r="N20" s="78" t="s">
         <v>13</v>
       </c>
-      <c r="O20" s="92" t="s">
+      <c r="O20" s="78" t="s">
         <v>287</v>
       </c>
-      <c r="P20" s="93" t="s">
+      <c r="P20" s="79" t="s">
         <v>61</v>
       </c>
-      <c r="Q20" s="94"/>
-      <c r="R20" s="95"/>
+      <c r="Q20" s="80"/>
+      <c r="R20" s="81"/>
       <c r="S20" s="35" t="s">
         <v>124</v>
       </c>
@@ -2956,13 +2947,13 @@
       <c r="AD20" s="3" t="s">
         <v>124</v>
       </c>
-      <c r="AE20" s="72" t="s">
-        <v>294</v>
-      </c>
-      <c r="AF20" s="72">
-        <v>1</v>
-      </c>
-      <c r="AG20" s="77" t="s">
+      <c r="AE20" s="64" t="s">
+        <v>294</v>
+      </c>
+      <c r="AF20" s="64">
+        <v>1</v>
+      </c>
+      <c r="AG20" s="68" t="s">
         <v>308</v>
       </c>
       <c r="AH20" s="3">
@@ -2981,10 +2972,10 @@
       <c r="AM20" s="1" t="s">
         <v>124</v>
       </c>
-      <c r="AN20" s="73" t="s">
-        <v>294</v>
-      </c>
-      <c r="AO20" s="68">
+      <c r="AN20" s="65" t="s">
+        <v>294</v>
+      </c>
+      <c r="AO20" s="61">
         <v>1</v>
       </c>
       <c r="AP20" s="1">
@@ -2993,25 +2984,25 @@
     </row>
     <row r="21" spans="2:42" x14ac:dyDescent="0.25">
       <c r="C21" s="41"/>
-      <c r="D21" s="63"/>
-      <c r="E21" s="70"/>
-      <c r="F21" s="70"/>
-      <c r="G21" s="70"/>
-      <c r="H21" s="70"/>
+      <c r="D21" s="56"/>
+      <c r="E21" s="62"/>
+      <c r="F21" s="62"/>
+      <c r="G21" s="62"/>
+      <c r="H21" s="62"/>
       <c r="M21" s="34" t="s">
         <v>40</v>
       </c>
-      <c r="N21" s="92" t="s">
+      <c r="N21" s="78" t="s">
         <v>13</v>
       </c>
-      <c r="O21" s="92" t="s">
+      <c r="O21" s="78" t="s">
         <v>287</v>
       </c>
-      <c r="P21" s="93" t="s">
+      <c r="P21" s="79" t="s">
         <v>61</v>
       </c>
-      <c r="Q21" s="94"/>
-      <c r="R21" s="95"/>
+      <c r="Q21" s="80"/>
+      <c r="R21" s="81"/>
       <c r="S21" s="35" t="s">
         <v>125</v>
       </c>
@@ -3045,13 +3036,13 @@
       <c r="AD21" s="3" t="s">
         <v>125</v>
       </c>
-      <c r="AE21" s="72" t="s">
-        <v>294</v>
-      </c>
-      <c r="AF21" s="72">
-        <v>1</v>
-      </c>
-      <c r="AG21" s="77" t="s">
+      <c r="AE21" s="64" t="s">
+        <v>294</v>
+      </c>
+      <c r="AF21" s="64">
+        <v>1</v>
+      </c>
+      <c r="AG21" s="68" t="s">
         <v>308</v>
       </c>
       <c r="AH21" s="3">
@@ -3070,10 +3061,10 @@
       <c r="AM21" s="1" t="s">
         <v>125</v>
       </c>
-      <c r="AN21" s="73" t="s">
-        <v>294</v>
-      </c>
-      <c r="AO21" s="68">
+      <c r="AN21" s="65" t="s">
+        <v>294</v>
+      </c>
+      <c r="AO21" s="61">
         <v>1</v>
       </c>
       <c r="AP21" s="1">
@@ -3082,25 +3073,25 @@
     </row>
     <row r="22" spans="2:42" x14ac:dyDescent="0.25">
       <c r="C22" s="41"/>
-      <c r="D22" s="63"/>
-      <c r="E22" s="70"/>
-      <c r="F22" s="70"/>
-      <c r="G22" s="70"/>
-      <c r="H22" s="70"/>
+      <c r="D22" s="56"/>
+      <c r="E22" s="62"/>
+      <c r="F22" s="62"/>
+      <c r="G22" s="62"/>
+      <c r="H22" s="62"/>
       <c r="M22" s="34" t="s">
         <v>41</v>
       </c>
-      <c r="N22" s="92" t="s">
+      <c r="N22" s="78" t="s">
         <v>13</v>
       </c>
-      <c r="O22" s="92" t="s">
+      <c r="O22" s="78" t="s">
         <v>287</v>
       </c>
-      <c r="P22" s="93" t="s">
+      <c r="P22" s="79" t="s">
         <v>61</v>
       </c>
-      <c r="Q22" s="94"/>
-      <c r="R22" s="95"/>
+      <c r="Q22" s="80"/>
+      <c r="R22" s="81"/>
       <c r="S22" s="35" t="s">
         <v>126</v>
       </c>
@@ -3134,13 +3125,13 @@
       <c r="AD22" s="3" t="s">
         <v>126</v>
       </c>
-      <c r="AE22" s="72" t="s">
-        <v>294</v>
-      </c>
-      <c r="AF22" s="72">
-        <v>1</v>
-      </c>
-      <c r="AG22" s="77" t="s">
+      <c r="AE22" s="64" t="s">
+        <v>294</v>
+      </c>
+      <c r="AF22" s="64">
+        <v>1</v>
+      </c>
+      <c r="AG22" s="68" t="s">
         <v>308</v>
       </c>
       <c r="AH22" s="3">
@@ -3159,10 +3150,10 @@
       <c r="AM22" s="1" t="s">
         <v>126</v>
       </c>
-      <c r="AN22" s="73" t="s">
-        <v>294</v>
-      </c>
-      <c r="AO22" s="68">
+      <c r="AN22" s="65" t="s">
+        <v>294</v>
+      </c>
+      <c r="AO22" s="61">
         <v>1</v>
       </c>
       <c r="AP22" s="1">
@@ -3171,25 +3162,25 @@
     </row>
     <row r="23" spans="2:42" x14ac:dyDescent="0.25">
       <c r="C23" s="41"/>
-      <c r="D23" s="63"/>
-      <c r="E23" s="70"/>
-      <c r="F23" s="70"/>
-      <c r="G23" s="70"/>
-      <c r="H23" s="70"/>
+      <c r="D23" s="56"/>
+      <c r="E23" s="62"/>
+      <c r="F23" s="62"/>
+      <c r="G23" s="62"/>
+      <c r="H23" s="62"/>
       <c r="M23" s="34" t="s">
         <v>42</v>
       </c>
-      <c r="N23" s="92" t="s">
+      <c r="N23" s="78" t="s">
         <v>13</v>
       </c>
-      <c r="O23" s="92" t="s">
+      <c r="O23" s="78" t="s">
         <v>287</v>
       </c>
-      <c r="P23" s="93" t="s">
+      <c r="P23" s="79" t="s">
         <v>61</v>
       </c>
-      <c r="Q23" s="94"/>
-      <c r="R23" s="95"/>
+      <c r="Q23" s="80"/>
+      <c r="R23" s="81"/>
       <c r="S23" s="35" t="s">
         <v>127</v>
       </c>
@@ -3223,13 +3214,13 @@
       <c r="AD23" s="3" t="s">
         <v>127</v>
       </c>
-      <c r="AE23" s="72" t="s">
-        <v>294</v>
-      </c>
-      <c r="AF23" s="72">
-        <v>1</v>
-      </c>
-      <c r="AG23" s="77" t="s">
+      <c r="AE23" s="64" t="s">
+        <v>294</v>
+      </c>
+      <c r="AF23" s="64">
+        <v>1</v>
+      </c>
+      <c r="AG23" s="68" t="s">
         <v>308</v>
       </c>
       <c r="AH23" s="3">
@@ -3247,10 +3238,10 @@
       <c r="AM23" s="1" t="s">
         <v>127</v>
       </c>
-      <c r="AN23" s="73" t="s">
-        <v>294</v>
-      </c>
-      <c r="AO23" s="68">
+      <c r="AN23" s="65" t="s">
+        <v>294</v>
+      </c>
+      <c r="AO23" s="61">
         <v>1</v>
       </c>
       <c r="AP23" s="1">
@@ -3290,31 +3281,31 @@
       <c r="Y24" s="1" t="s">
         <v>306</v>
       </c>
-      <c r="AA24" s="72" t="s">
+      <c r="AA24" s="64" t="s">
         <v>216</v>
       </c>
-      <c r="AB24" s="85" t="s">
+      <c r="AB24" s="74" t="s">
         <v>178</v>
       </c>
-      <c r="AC24" s="72" t="s">
+      <c r="AC24" s="64" t="s">
         <v>14</v>
       </c>
-      <c r="AD24" s="86" t="s">
+      <c r="AD24" s="75" t="s">
         <v>72</v>
       </c>
-      <c r="AE24" s="72" t="s">
-        <v>294</v>
-      </c>
-      <c r="AF24" s="72">
-        <v>1</v>
-      </c>
-      <c r="AG24" s="77" t="s">
+      <c r="AE24" s="64" t="s">
+        <v>294</v>
+      </c>
+      <c r="AF24" s="64">
+        <v>1</v>
+      </c>
+      <c r="AG24" s="68" t="s">
         <v>308</v>
       </c>
-      <c r="AH24" s="72">
+      <c r="AH24" s="64">
         <v>70000</v>
       </c>
-      <c r="AI24" s="65"/>
+      <c r="AI24" s="58"/>
       <c r="AJ24" s="1" t="s">
         <v>245</v>
       </c>
@@ -3327,10 +3318,10 @@
       <c r="AM24" s="1" t="s">
         <v>72</v>
       </c>
-      <c r="AN24" s="73" t="s">
-        <v>294</v>
-      </c>
-      <c r="AO24" s="68">
+      <c r="AN24" s="65" t="s">
+        <v>294</v>
+      </c>
+      <c r="AO24" s="61">
         <v>1</v>
       </c>
       <c r="AP24" s="1">
@@ -3369,31 +3360,31 @@
       <c r="Y25" s="1" t="s">
         <v>306</v>
       </c>
-      <c r="AA25" s="72" t="s">
+      <c r="AA25" s="64" t="s">
         <v>217</v>
       </c>
-      <c r="AB25" s="85" t="s">
+      <c r="AB25" s="74" t="s">
         <v>178</v>
       </c>
-      <c r="AC25" s="72" t="s">
+      <c r="AC25" s="64" t="s">
         <v>14</v>
       </c>
-      <c r="AD25" s="72" t="s">
+      <c r="AD25" s="64" t="s">
         <v>160</v>
       </c>
-      <c r="AE25" s="72" t="s">
-        <v>294</v>
-      </c>
-      <c r="AF25" s="72">
-        <v>1</v>
-      </c>
-      <c r="AG25" s="77" t="s">
+      <c r="AE25" s="64" t="s">
+        <v>294</v>
+      </c>
+      <c r="AF25" s="64">
+        <v>1</v>
+      </c>
+      <c r="AG25" s="68" t="s">
         <v>308</v>
       </c>
-      <c r="AH25" s="72">
+      <c r="AH25" s="64">
         <v>70000</v>
       </c>
-      <c r="AI25" s="65"/>
+      <c r="AI25" s="58"/>
       <c r="AJ25" s="1" t="s">
         <v>246</v>
       </c>
@@ -3406,10 +3397,10 @@
       <c r="AM25" s="1" t="s">
         <v>160</v>
       </c>
-      <c r="AN25" s="73" t="s">
-        <v>294</v>
-      </c>
-      <c r="AO25" s="68">
+      <c r="AN25" s="65" t="s">
+        <v>294</v>
+      </c>
+      <c r="AO25" s="61">
         <v>1</v>
       </c>
       <c r="AP25" s="1">
@@ -3448,31 +3439,31 @@
       <c r="Y26" s="1" t="s">
         <v>306</v>
       </c>
-      <c r="AA26" s="72" t="s">
+      <c r="AA26" s="64" t="s">
         <v>218</v>
       </c>
-      <c r="AB26" s="85" t="s">
+      <c r="AB26" s="74" t="s">
         <v>178</v>
       </c>
-      <c r="AC26" s="72" t="s">
+      <c r="AC26" s="64" t="s">
         <v>14</v>
       </c>
-      <c r="AD26" s="72" t="s">
+      <c r="AD26" s="64" t="s">
         <v>161</v>
       </c>
-      <c r="AE26" s="72" t="s">
-        <v>294</v>
-      </c>
-      <c r="AF26" s="72">
-        <v>1</v>
-      </c>
-      <c r="AG26" s="77" t="s">
+      <c r="AE26" s="64" t="s">
+        <v>294</v>
+      </c>
+      <c r="AF26" s="64">
+        <v>1</v>
+      </c>
+      <c r="AG26" s="68" t="s">
         <v>308</v>
       </c>
-      <c r="AH26" s="72">
+      <c r="AH26" s="64">
         <v>70000</v>
       </c>
-      <c r="AI26" s="65"/>
+      <c r="AI26" s="58"/>
       <c r="AJ26" s="1" t="s">
         <v>247</v>
       </c>
@@ -3485,10 +3476,10 @@
       <c r="AM26" s="1" t="s">
         <v>161</v>
       </c>
-      <c r="AN26" s="73" t="s">
-        <v>294</v>
-      </c>
-      <c r="AO26" s="68">
+      <c r="AN26" s="65" t="s">
+        <v>294</v>
+      </c>
+      <c r="AO26" s="61">
         <v>1</v>
       </c>
       <c r="AP26" s="1">
@@ -3527,31 +3518,31 @@
       <c r="Y27" s="1" t="s">
         <v>306</v>
       </c>
-      <c r="AA27" s="72" t="s">
+      <c r="AA27" s="64" t="s">
         <v>219</v>
       </c>
-      <c r="AB27" s="85" t="s">
+      <c r="AB27" s="74" t="s">
         <v>178</v>
       </c>
-      <c r="AC27" s="72" t="s">
+      <c r="AC27" s="64" t="s">
         <v>14</v>
       </c>
-      <c r="AD27" s="72" t="s">
+      <c r="AD27" s="64" t="s">
         <v>162</v>
       </c>
-      <c r="AE27" s="72" t="s">
-        <v>294</v>
-      </c>
-      <c r="AF27" s="72">
-        <v>1</v>
-      </c>
-      <c r="AG27" s="77" t="s">
+      <c r="AE27" s="64" t="s">
+        <v>294</v>
+      </c>
+      <c r="AF27" s="64">
+        <v>1</v>
+      </c>
+      <c r="AG27" s="68" t="s">
         <v>308</v>
       </c>
-      <c r="AH27" s="72">
+      <c r="AH27" s="64">
         <v>70000</v>
       </c>
-      <c r="AI27" s="65"/>
+      <c r="AI27" s="58"/>
       <c r="AJ27" s="1" t="s">
         <v>248</v>
       </c>
@@ -3564,10 +3555,10 @@
       <c r="AM27" s="1" t="s">
         <v>162</v>
       </c>
-      <c r="AN27" s="73" t="s">
-        <v>294</v>
-      </c>
-      <c r="AO27" s="68">
+      <c r="AN27" s="65" t="s">
+        <v>294</v>
+      </c>
+      <c r="AO27" s="61">
         <v>1</v>
       </c>
       <c r="AP27" s="1">
@@ -3606,31 +3597,31 @@
       <c r="Y28" s="1" t="s">
         <v>306</v>
       </c>
-      <c r="AA28" s="72" t="s">
+      <c r="AA28" s="64" t="s">
         <v>220</v>
       </c>
-      <c r="AB28" s="85" t="s">
+      <c r="AB28" s="74" t="s">
         <v>178</v>
       </c>
-      <c r="AC28" s="72" t="s">
+      <c r="AC28" s="64" t="s">
         <v>14</v>
       </c>
-      <c r="AD28" s="72" t="s">
+      <c r="AD28" s="64" t="s">
         <v>163</v>
       </c>
-      <c r="AE28" s="72" t="s">
-        <v>294</v>
-      </c>
-      <c r="AF28" s="72">
-        <v>1</v>
-      </c>
-      <c r="AG28" s="77" t="s">
+      <c r="AE28" s="64" t="s">
+        <v>294</v>
+      </c>
+      <c r="AF28" s="64">
+        <v>1</v>
+      </c>
+      <c r="AG28" s="68" t="s">
         <v>308</v>
       </c>
-      <c r="AH28" s="72">
+      <c r="AH28" s="64">
         <v>70000</v>
       </c>
-      <c r="AI28" s="65"/>
+      <c r="AI28" s="58"/>
       <c r="AJ28" s="1" t="s">
         <v>249</v>
       </c>
@@ -3643,10 +3634,10 @@
       <c r="AM28" s="1" t="s">
         <v>163</v>
       </c>
-      <c r="AN28" s="73" t="s">
-        <v>294</v>
-      </c>
-      <c r="AO28" s="68">
+      <c r="AN28" s="65" t="s">
+        <v>294</v>
+      </c>
+      <c r="AO28" s="61">
         <v>1</v>
       </c>
       <c r="AP28" s="1">
@@ -3685,31 +3676,31 @@
       <c r="Y29" s="1" t="s">
         <v>306</v>
       </c>
-      <c r="AA29" s="72" t="s">
+      <c r="AA29" s="64" t="s">
         <v>221</v>
       </c>
-      <c r="AB29" s="85" t="s">
+      <c r="AB29" s="74" t="s">
         <v>178</v>
       </c>
-      <c r="AC29" s="87" t="s">
+      <c r="AC29" s="76" t="s">
         <v>15</v>
       </c>
-      <c r="AD29" s="88" t="s">
+      <c r="AD29" s="77" t="s">
         <v>73</v>
       </c>
-      <c r="AE29" s="72" t="s">
-        <v>294</v>
-      </c>
-      <c r="AF29" s="72">
-        <v>1</v>
-      </c>
-      <c r="AG29" s="77" t="s">
+      <c r="AE29" s="64" t="s">
+        <v>294</v>
+      </c>
+      <c r="AF29" s="64">
+        <v>1</v>
+      </c>
+      <c r="AG29" s="68" t="s">
         <v>308</v>
       </c>
-      <c r="AH29" s="72">
+      <c r="AH29" s="64">
         <v>70000</v>
       </c>
-      <c r="AI29" s="65"/>
+      <c r="AI29" s="58"/>
       <c r="AJ29" s="1" t="s">
         <v>250</v>
       </c>
@@ -3722,10 +3713,10 @@
       <c r="AM29" s="1" t="s">
         <v>73</v>
       </c>
-      <c r="AN29" s="73" t="s">
-        <v>294</v>
-      </c>
-      <c r="AO29" s="68">
+      <c r="AN29" s="65" t="s">
+        <v>294</v>
+      </c>
+      <c r="AO29" s="61">
         <v>1</v>
       </c>
       <c r="AP29" s="1">
@@ -3764,31 +3755,31 @@
       <c r="Y30" s="1" t="s">
         <v>306</v>
       </c>
-      <c r="AA30" s="72" t="s">
+      <c r="AA30" s="64" t="s">
         <v>222</v>
       </c>
-      <c r="AB30" s="85" t="s">
+      <c r="AB30" s="74" t="s">
         <v>178</v>
       </c>
-      <c r="AC30" s="87" t="s">
+      <c r="AC30" s="76" t="s">
         <v>15</v>
       </c>
-      <c r="AD30" s="88" t="s">
+      <c r="AD30" s="77" t="s">
         <v>165</v>
       </c>
-      <c r="AE30" s="72" t="s">
-        <v>294</v>
-      </c>
-      <c r="AF30" s="72">
-        <v>1</v>
-      </c>
-      <c r="AG30" s="77" t="s">
+      <c r="AE30" s="64" t="s">
+        <v>294</v>
+      </c>
+      <c r="AF30" s="64">
+        <v>1</v>
+      </c>
+      <c r="AG30" s="68" t="s">
         <v>308</v>
       </c>
-      <c r="AH30" s="72">
+      <c r="AH30" s="64">
         <v>70000</v>
       </c>
-      <c r="AI30" s="65"/>
+      <c r="AI30" s="58"/>
       <c r="AJ30" s="1" t="s">
         <v>251</v>
       </c>
@@ -3801,10 +3792,10 @@
       <c r="AM30" s="1" t="s">
         <v>165</v>
       </c>
-      <c r="AN30" s="73" t="s">
-        <v>294</v>
-      </c>
-      <c r="AO30" s="68">
+      <c r="AN30" s="65" t="s">
+        <v>294</v>
+      </c>
+      <c r="AO30" s="61">
         <v>1</v>
       </c>
       <c r="AP30" s="1">
@@ -3843,31 +3834,31 @@
       <c r="Y31" s="1" t="s">
         <v>306</v>
       </c>
-      <c r="AA31" s="72" t="s">
+      <c r="AA31" s="64" t="s">
         <v>223</v>
       </c>
-      <c r="AB31" s="85" t="s">
+      <c r="AB31" s="74" t="s">
         <v>178</v>
       </c>
-      <c r="AC31" s="87" t="s">
+      <c r="AC31" s="76" t="s">
         <v>15</v>
       </c>
-      <c r="AD31" s="88" t="s">
+      <c r="AD31" s="77" t="s">
         <v>166</v>
       </c>
-      <c r="AE31" s="72" t="s">
-        <v>294</v>
-      </c>
-      <c r="AF31" s="72">
-        <v>1</v>
-      </c>
-      <c r="AG31" s="77" t="s">
+      <c r="AE31" s="64" t="s">
+        <v>294</v>
+      </c>
+      <c r="AF31" s="64">
+        <v>1</v>
+      </c>
+      <c r="AG31" s="68" t="s">
         <v>308</v>
       </c>
-      <c r="AH31" s="72">
+      <c r="AH31" s="64">
         <v>70000</v>
       </c>
-      <c r="AI31" s="65"/>
+      <c r="AI31" s="58"/>
       <c r="AJ31" s="1" t="s">
         <v>252</v>
       </c>
@@ -3880,10 +3871,10 @@
       <c r="AM31" s="1" t="s">
         <v>166</v>
       </c>
-      <c r="AN31" s="73" t="s">
-        <v>294</v>
-      </c>
-      <c r="AO31" s="68">
+      <c r="AN31" s="65" t="s">
+        <v>294</v>
+      </c>
+      <c r="AO31" s="61">
         <v>1</v>
       </c>
       <c r="AP31" s="1">
@@ -3922,31 +3913,31 @@
       <c r="Y32" s="1" t="s">
         <v>306</v>
       </c>
-      <c r="AA32" s="72" t="s">
+      <c r="AA32" s="64" t="s">
         <v>224</v>
       </c>
-      <c r="AB32" s="85" t="s">
+      <c r="AB32" s="74" t="s">
         <v>178</v>
       </c>
-      <c r="AC32" s="87" t="s">
+      <c r="AC32" s="76" t="s">
         <v>16</v>
       </c>
-      <c r="AD32" s="88" t="s">
+      <c r="AD32" s="77" t="s">
         <v>70</v>
       </c>
-      <c r="AE32" s="72" t="s">
-        <v>294</v>
-      </c>
-      <c r="AF32" s="72">
-        <v>1</v>
-      </c>
-      <c r="AG32" s="77" t="s">
+      <c r="AE32" s="64" t="s">
+        <v>294</v>
+      </c>
+      <c r="AF32" s="64">
+        <v>1</v>
+      </c>
+      <c r="AG32" s="68" t="s">
         <v>308</v>
       </c>
-      <c r="AH32" s="72">
+      <c r="AH32" s="64">
         <v>70000</v>
       </c>
-      <c r="AI32" s="65"/>
+      <c r="AI32" s="58"/>
       <c r="AJ32" s="1" t="s">
         <v>253</v>
       </c>
@@ -3959,10 +3950,10 @@
       <c r="AM32" s="1" t="s">
         <v>70</v>
       </c>
-      <c r="AN32" s="73" t="s">
-        <v>294</v>
-      </c>
-      <c r="AO32" s="68">
+      <c r="AN32" s="65" t="s">
+        <v>294</v>
+      </c>
+      <c r="AO32" s="61">
         <v>1</v>
       </c>
       <c r="AP32" s="1">
@@ -4001,31 +3992,31 @@
       <c r="Y33" s="1" t="s">
         <v>306</v>
       </c>
-      <c r="AA33" s="72" t="s">
+      <c r="AA33" s="64" t="s">
         <v>225</v>
       </c>
-      <c r="AB33" s="85" t="s">
+      <c r="AB33" s="74" t="s">
         <v>178</v>
       </c>
-      <c r="AC33" s="87" t="s">
+      <c r="AC33" s="76" t="s">
         <v>16</v>
       </c>
-      <c r="AD33" s="88" t="s">
+      <c r="AD33" s="77" t="s">
         <v>71</v>
       </c>
-      <c r="AE33" s="72" t="s">
-        <v>294</v>
-      </c>
-      <c r="AF33" s="72">
-        <v>1</v>
-      </c>
-      <c r="AG33" s="77" t="s">
+      <c r="AE33" s="64" t="s">
+        <v>294</v>
+      </c>
+      <c r="AF33" s="64">
+        <v>1</v>
+      </c>
+      <c r="AG33" s="68" t="s">
         <v>308</v>
       </c>
-      <c r="AH33" s="72">
+      <c r="AH33" s="64">
         <v>70000</v>
       </c>
-      <c r="AI33" s="65"/>
+      <c r="AI33" s="58"/>
       <c r="AJ33" s="1" t="s">
         <v>254</v>
       </c>
@@ -4038,10 +4029,10 @@
       <c r="AM33" s="1" t="s">
         <v>71</v>
       </c>
-      <c r="AN33" s="73" t="s">
-        <v>294</v>
-      </c>
-      <c r="AO33" s="68">
+      <c r="AN33" s="65" t="s">
+        <v>294</v>
+      </c>
+      <c r="AO33" s="61">
         <v>1</v>
       </c>
       <c r="AP33" s="1">
@@ -4080,31 +4071,31 @@
       <c r="Y34" s="1" t="s">
         <v>306</v>
       </c>
-      <c r="AA34" s="72" t="s">
+      <c r="AA34" s="64" t="s">
         <v>226</v>
       </c>
-      <c r="AB34" s="85" t="s">
+      <c r="AB34" s="74" t="s">
         <v>178</v>
       </c>
-      <c r="AC34" s="87" t="s">
+      <c r="AC34" s="76" t="s">
         <v>16</v>
       </c>
-      <c r="AD34" s="88" t="s">
+      <c r="AD34" s="77" t="s">
         <v>72</v>
       </c>
-      <c r="AE34" s="72" t="s">
-        <v>294</v>
-      </c>
-      <c r="AF34" s="72">
-        <v>1</v>
-      </c>
-      <c r="AG34" s="77" t="s">
+      <c r="AE34" s="64" t="s">
+        <v>294</v>
+      </c>
+      <c r="AF34" s="64">
+        <v>1</v>
+      </c>
+      <c r="AG34" s="68" t="s">
         <v>308</v>
       </c>
-      <c r="AH34" s="72">
+      <c r="AH34" s="64">
         <v>70000</v>
       </c>
-      <c r="AI34" s="65"/>
+      <c r="AI34" s="58"/>
       <c r="AJ34" s="1" t="s">
         <v>255</v>
       </c>
@@ -4117,10 +4108,10 @@
       <c r="AM34" s="1" t="s">
         <v>72</v>
       </c>
-      <c r="AN34" s="73" t="s">
-        <v>294</v>
-      </c>
-      <c r="AO34" s="68">
+      <c r="AN34" s="65" t="s">
+        <v>294</v>
+      </c>
+      <c r="AO34" s="61">
         <v>1</v>
       </c>
       <c r="AP34" s="1">
@@ -4159,31 +4150,31 @@
       <c r="Y35" s="1" t="s">
         <v>306</v>
       </c>
-      <c r="AA35" s="72" t="s">
+      <c r="AA35" s="64" t="s">
         <v>227</v>
       </c>
-      <c r="AB35" s="85" t="s">
+      <c r="AB35" s="74" t="s">
         <v>178</v>
       </c>
-      <c r="AC35" s="87" t="s">
+      <c r="AC35" s="76" t="s">
         <v>16</v>
       </c>
-      <c r="AD35" s="88" t="s">
+      <c r="AD35" s="77" t="s">
         <v>73</v>
       </c>
-      <c r="AE35" s="72" t="s">
-        <v>294</v>
-      </c>
-      <c r="AF35" s="72">
-        <v>1</v>
-      </c>
-      <c r="AG35" s="77" t="s">
+      <c r="AE35" s="64" t="s">
+        <v>294</v>
+      </c>
+      <c r="AF35" s="64">
+        <v>1</v>
+      </c>
+      <c r="AG35" s="68" t="s">
         <v>308</v>
       </c>
-      <c r="AH35" s="72">
+      <c r="AH35" s="64">
         <v>70000</v>
       </c>
-      <c r="AI35" s="65"/>
+      <c r="AI35" s="58"/>
       <c r="AJ35" s="1" t="s">
         <v>256</v>
       </c>
@@ -4196,10 +4187,10 @@
       <c r="AM35" s="1" t="s">
         <v>73</v>
       </c>
-      <c r="AN35" s="73" t="s">
-        <v>294</v>
-      </c>
-      <c r="AO35" s="68">
+      <c r="AN35" s="65" t="s">
+        <v>294</v>
+      </c>
+      <c r="AO35" s="61">
         <v>1</v>
       </c>
       <c r="AP35" s="1">
@@ -4238,31 +4229,31 @@
       <c r="Y36" s="1" t="s">
         <v>306</v>
       </c>
-      <c r="AA36" s="72" t="s">
+      <c r="AA36" s="64" t="s">
         <v>228</v>
       </c>
-      <c r="AB36" s="85" t="s">
+      <c r="AB36" s="74" t="s">
         <v>178</v>
       </c>
-      <c r="AC36" s="87" t="s">
+      <c r="AC36" s="76" t="s">
         <v>17</v>
       </c>
-      <c r="AD36" s="88" t="s">
+      <c r="AD36" s="77" t="s">
         <v>160</v>
       </c>
-      <c r="AE36" s="72" t="s">
-        <v>294</v>
-      </c>
-      <c r="AF36" s="72">
-        <v>1</v>
-      </c>
-      <c r="AG36" s="77" t="s">
+      <c r="AE36" s="64" t="s">
+        <v>294</v>
+      </c>
+      <c r="AF36" s="64">
+        <v>1</v>
+      </c>
+      <c r="AG36" s="68" t="s">
         <v>308</v>
       </c>
-      <c r="AH36" s="72">
+      <c r="AH36" s="64">
         <v>70000</v>
       </c>
-      <c r="AI36" s="65"/>
+      <c r="AI36" s="58"/>
       <c r="AJ36" s="1" t="s">
         <v>257</v>
       </c>
@@ -4275,10 +4266,10 @@
       <c r="AM36" s="1" t="s">
         <v>160</v>
       </c>
-      <c r="AN36" s="73" t="s">
-        <v>294</v>
-      </c>
-      <c r="AO36" s="68">
+      <c r="AN36" s="65" t="s">
+        <v>294</v>
+      </c>
+      <c r="AO36" s="61">
         <v>1</v>
       </c>
       <c r="AP36" s="1">
@@ -4317,31 +4308,31 @@
       <c r="Y37" s="1" t="s">
         <v>306</v>
       </c>
-      <c r="AA37" s="72" t="s">
+      <c r="AA37" s="64" t="s">
         <v>229</v>
       </c>
-      <c r="AB37" s="85" t="s">
+      <c r="AB37" s="74" t="s">
         <v>178</v>
       </c>
-      <c r="AC37" s="87" t="s">
+      <c r="AC37" s="76" t="s">
         <v>17</v>
       </c>
-      <c r="AD37" s="88" t="s">
+      <c r="AD37" s="77" t="s">
         <v>161</v>
       </c>
-      <c r="AE37" s="72" t="s">
-        <v>294</v>
-      </c>
-      <c r="AF37" s="72">
-        <v>1</v>
-      </c>
-      <c r="AG37" s="77" t="s">
+      <c r="AE37" s="64" t="s">
+        <v>294</v>
+      </c>
+      <c r="AF37" s="64">
+        <v>1</v>
+      </c>
+      <c r="AG37" s="68" t="s">
         <v>308</v>
       </c>
-      <c r="AH37" s="72">
+      <c r="AH37" s="64">
         <v>70000</v>
       </c>
-      <c r="AI37" s="65"/>
+      <c r="AI37" s="58"/>
       <c r="AJ37" s="1" t="s">
         <v>258</v>
       </c>
@@ -4354,10 +4345,10 @@
       <c r="AM37" s="1" t="s">
         <v>161</v>
       </c>
-      <c r="AN37" s="73" t="s">
-        <v>294</v>
-      </c>
-      <c r="AO37" s="68">
+      <c r="AN37" s="65" t="s">
+        <v>294</v>
+      </c>
+      <c r="AO37" s="61">
         <v>1</v>
       </c>
       <c r="AP37" s="1">
@@ -4396,31 +4387,31 @@
       <c r="Y38" s="1" t="s">
         <v>306</v>
       </c>
-      <c r="AA38" s="72" t="s">
+      <c r="AA38" s="64" t="s">
         <v>230</v>
       </c>
-      <c r="AB38" s="85" t="s">
+      <c r="AB38" s="74" t="s">
         <v>178</v>
       </c>
-      <c r="AC38" s="87" t="s">
+      <c r="AC38" s="76" t="s">
         <v>17</v>
       </c>
-      <c r="AD38" s="88" t="s">
+      <c r="AD38" s="77" t="s">
         <v>162</v>
       </c>
-      <c r="AE38" s="72" t="s">
-        <v>294</v>
-      </c>
-      <c r="AF38" s="72">
-        <v>1</v>
-      </c>
-      <c r="AG38" s="77" t="s">
+      <c r="AE38" s="64" t="s">
+        <v>294</v>
+      </c>
+      <c r="AF38" s="64">
+        <v>1</v>
+      </c>
+      <c r="AG38" s="68" t="s">
         <v>308</v>
       </c>
-      <c r="AH38" s="72">
+      <c r="AH38" s="64">
         <v>70000</v>
       </c>
-      <c r="AI38" s="65"/>
+      <c r="AI38" s="58"/>
       <c r="AJ38" s="1" t="s">
         <v>259</v>
       </c>
@@ -4433,10 +4424,10 @@
       <c r="AM38" s="1" t="s">
         <v>162</v>
       </c>
-      <c r="AN38" s="73" t="s">
-        <v>294</v>
-      </c>
-      <c r="AO38" s="68">
+      <c r="AN38" s="65" t="s">
+        <v>294</v>
+      </c>
+      <c r="AO38" s="61">
         <v>1</v>
       </c>
       <c r="AP38" s="1">
@@ -4475,31 +4466,31 @@
       <c r="Y39" s="1" t="s">
         <v>306</v>
       </c>
-      <c r="AA39" s="72" t="s">
+      <c r="AA39" s="64" t="s">
         <v>231</v>
       </c>
-      <c r="AB39" s="85" t="s">
+      <c r="AB39" s="74" t="s">
         <v>178</v>
       </c>
-      <c r="AC39" s="87" t="s">
+      <c r="AC39" s="76" t="s">
         <v>17</v>
       </c>
-      <c r="AD39" s="88" t="s">
+      <c r="AD39" s="77" t="s">
         <v>163</v>
       </c>
-      <c r="AE39" s="72" t="s">
-        <v>294</v>
-      </c>
-      <c r="AF39" s="72">
-        <v>1</v>
-      </c>
-      <c r="AG39" s="77" t="s">
+      <c r="AE39" s="64" t="s">
+        <v>294</v>
+      </c>
+      <c r="AF39" s="64">
+        <v>1</v>
+      </c>
+      <c r="AG39" s="68" t="s">
         <v>308</v>
       </c>
-      <c r="AH39" s="72">
+      <c r="AH39" s="64">
         <v>70000</v>
       </c>
-      <c r="AI39" s="65"/>
+      <c r="AI39" s="58"/>
       <c r="AJ39" s="1" t="s">
         <v>260</v>
       </c>
@@ -4512,10 +4503,10 @@
       <c r="AM39" s="1" t="s">
         <v>163</v>
       </c>
-      <c r="AN39" s="73" t="s">
-        <v>294</v>
-      </c>
-      <c r="AO39" s="68">
+      <c r="AN39" s="65" t="s">
+        <v>294</v>
+      </c>
+      <c r="AO39" s="61">
         <v>1</v>
       </c>
       <c r="AP39" s="1">
@@ -4554,31 +4545,31 @@
       <c r="Y40" s="1" t="s">
         <v>306</v>
       </c>
-      <c r="AA40" s="72" t="s">
+      <c r="AA40" s="64" t="s">
         <v>232</v>
       </c>
-      <c r="AB40" s="85" t="s">
+      <c r="AB40" s="74" t="s">
         <v>178</v>
       </c>
-      <c r="AC40" s="87" t="s">
+      <c r="AC40" s="76" t="s">
         <v>18</v>
       </c>
-      <c r="AD40" s="88" t="s">
+      <c r="AD40" s="77" t="s">
         <v>120</v>
       </c>
-      <c r="AE40" s="72" t="s">
-        <v>294</v>
-      </c>
-      <c r="AF40" s="72">
-        <v>1</v>
-      </c>
-      <c r="AG40" s="77" t="s">
+      <c r="AE40" s="64" t="s">
+        <v>294</v>
+      </c>
+      <c r="AF40" s="64">
+        <v>1</v>
+      </c>
+      <c r="AG40" s="68" t="s">
         <v>308</v>
       </c>
-      <c r="AH40" s="72">
+      <c r="AH40" s="64">
         <v>70000</v>
       </c>
-      <c r="AI40" s="65"/>
+      <c r="AI40" s="58"/>
       <c r="AJ40" s="1" t="s">
         <v>261</v>
       </c>
@@ -4591,10 +4582,10 @@
       <c r="AM40" s="1" t="s">
         <v>120</v>
       </c>
-      <c r="AN40" s="73" t="s">
-        <v>294</v>
-      </c>
-      <c r="AO40" s="68">
+      <c r="AN40" s="65" t="s">
+        <v>294</v>
+      </c>
+      <c r="AO40" s="61">
         <v>1</v>
       </c>
       <c r="AP40" s="1">
@@ -4633,31 +4624,31 @@
       <c r="Y41" s="1" t="s">
         <v>306</v>
       </c>
-      <c r="AA41" s="72" t="s">
+      <c r="AA41" s="64" t="s">
         <v>233</v>
       </c>
-      <c r="AB41" s="85" t="s">
+      <c r="AB41" s="74" t="s">
         <v>178</v>
       </c>
-      <c r="AC41" s="87" t="s">
+      <c r="AC41" s="76" t="s">
         <v>18</v>
       </c>
-      <c r="AD41" s="88" t="s">
+      <c r="AD41" s="77" t="s">
         <v>121</v>
       </c>
-      <c r="AE41" s="72" t="s">
-        <v>294</v>
-      </c>
-      <c r="AF41" s="72">
-        <v>1</v>
-      </c>
-      <c r="AG41" s="77" t="s">
+      <c r="AE41" s="64" t="s">
+        <v>294</v>
+      </c>
+      <c r="AF41" s="64">
+        <v>1</v>
+      </c>
+      <c r="AG41" s="68" t="s">
         <v>308</v>
       </c>
-      <c r="AH41" s="72">
+      <c r="AH41" s="64">
         <v>70000</v>
       </c>
-      <c r="AI41" s="65"/>
+      <c r="AI41" s="58"/>
       <c r="AJ41" s="1" t="s">
         <v>262</v>
       </c>
@@ -4670,10 +4661,10 @@
       <c r="AM41" s="1" t="s">
         <v>121</v>
       </c>
-      <c r="AN41" s="73" t="s">
-        <v>294</v>
-      </c>
-      <c r="AO41" s="68">
+      <c r="AN41" s="65" t="s">
+        <v>294</v>
+      </c>
+      <c r="AO41" s="61">
         <v>1</v>
       </c>
       <c r="AP41" s="1">
@@ -4712,31 +4703,31 @@
       <c r="Y42" s="1" t="s">
         <v>306</v>
       </c>
-      <c r="AA42" s="72" t="s">
+      <c r="AA42" s="64" t="s">
         <v>234</v>
       </c>
-      <c r="AB42" s="85" t="s">
+      <c r="AB42" s="74" t="s">
         <v>178</v>
       </c>
-      <c r="AC42" s="87" t="s">
+      <c r="AC42" s="76" t="s">
         <v>18</v>
       </c>
-      <c r="AD42" s="88" t="s">
+      <c r="AD42" s="77" t="s">
         <v>122</v>
       </c>
-      <c r="AE42" s="72" t="s">
-        <v>294</v>
-      </c>
-      <c r="AF42" s="72">
-        <v>1</v>
-      </c>
-      <c r="AG42" s="77" t="s">
+      <c r="AE42" s="64" t="s">
+        <v>294</v>
+      </c>
+      <c r="AF42" s="64">
+        <v>1</v>
+      </c>
+      <c r="AG42" s="68" t="s">
         <v>308</v>
       </c>
-      <c r="AH42" s="72">
+      <c r="AH42" s="64">
         <v>70000</v>
       </c>
-      <c r="AI42" s="65"/>
+      <c r="AI42" s="58"/>
       <c r="AJ42" s="1" t="s">
         <v>263</v>
       </c>
@@ -4749,10 +4740,10 @@
       <c r="AM42" s="1" t="s">
         <v>122</v>
       </c>
-      <c r="AN42" s="73" t="s">
-        <v>294</v>
-      </c>
-      <c r="AO42" s="68">
+      <c r="AN42" s="65" t="s">
+        <v>294</v>
+      </c>
+      <c r="AO42" s="61">
         <v>1</v>
       </c>
       <c r="AP42" s="1">
@@ -4791,31 +4782,31 @@
       <c r="Y43" s="1" t="s">
         <v>306</v>
       </c>
-      <c r="AA43" s="72" t="s">
+      <c r="AA43" s="64" t="s">
         <v>235</v>
       </c>
-      <c r="AB43" s="85" t="s">
+      <c r="AB43" s="74" t="s">
         <v>178</v>
       </c>
-      <c r="AC43" s="87" t="s">
+      <c r="AC43" s="76" t="s">
         <v>18</v>
       </c>
-      <c r="AD43" s="88" t="s">
+      <c r="AD43" s="77" t="s">
         <v>123</v>
       </c>
-      <c r="AE43" s="72" t="s">
-        <v>294</v>
-      </c>
-      <c r="AF43" s="72">
-        <v>1</v>
-      </c>
-      <c r="AG43" s="77" t="s">
+      <c r="AE43" s="64" t="s">
+        <v>294</v>
+      </c>
+      <c r="AF43" s="64">
+        <v>1</v>
+      </c>
+      <c r="AG43" s="68" t="s">
         <v>308</v>
       </c>
-      <c r="AH43" s="72">
+      <c r="AH43" s="64">
         <v>70000</v>
       </c>
-      <c r="AI43" s="65"/>
+      <c r="AI43" s="58"/>
       <c r="AJ43" s="1" t="s">
         <v>264</v>
       </c>
@@ -4828,10 +4819,10 @@
       <c r="AM43" s="1" t="s">
         <v>123</v>
       </c>
-      <c r="AN43" s="73" t="s">
-        <v>294</v>
-      </c>
-      <c r="AO43" s="68">
+      <c r="AN43" s="65" t="s">
+        <v>294</v>
+      </c>
+      <c r="AO43" s="61">
         <v>1</v>
       </c>
       <c r="AP43" s="1">
@@ -4870,31 +4861,31 @@
       <c r="Y44" s="1" t="s">
         <v>306</v>
       </c>
-      <c r="AA44" s="72" t="s">
+      <c r="AA44" s="64" t="s">
         <v>236</v>
       </c>
-      <c r="AB44" s="85" t="s">
+      <c r="AB44" s="74" t="s">
         <v>178</v>
       </c>
-      <c r="AC44" s="87" t="s">
+      <c r="AC44" s="76" t="s">
         <v>18</v>
       </c>
-      <c r="AD44" s="88" t="s">
+      <c r="AD44" s="77" t="s">
         <v>124</v>
       </c>
-      <c r="AE44" s="72" t="s">
-        <v>294</v>
-      </c>
-      <c r="AF44" s="72">
-        <v>1</v>
-      </c>
-      <c r="AG44" s="77" t="s">
+      <c r="AE44" s="64" t="s">
+        <v>294</v>
+      </c>
+      <c r="AF44" s="64">
+        <v>1</v>
+      </c>
+      <c r="AG44" s="68" t="s">
         <v>308</v>
       </c>
-      <c r="AH44" s="72">
+      <c r="AH44" s="64">
         <v>70000</v>
       </c>
-      <c r="AI44" s="65"/>
+      <c r="AI44" s="58"/>
       <c r="AJ44" s="1" t="s">
         <v>265</v>
       </c>
@@ -4907,10 +4898,10 @@
       <c r="AM44" s="1" t="s">
         <v>124</v>
       </c>
-      <c r="AN44" s="73" t="s">
-        <v>294</v>
-      </c>
-      <c r="AO44" s="68">
+      <c r="AN44" s="65" t="s">
+        <v>294</v>
+      </c>
+      <c r="AO44" s="61">
         <v>1</v>
       </c>
       <c r="AP44" s="1">
@@ -4949,31 +4940,31 @@
       <c r="Y45" s="1" t="s">
         <v>306</v>
       </c>
-      <c r="AA45" s="72" t="s">
+      <c r="AA45" s="64" t="s">
         <v>237</v>
       </c>
-      <c r="AB45" s="85" t="s">
+      <c r="AB45" s="74" t="s">
         <v>178</v>
       </c>
-      <c r="AC45" s="87" t="s">
+      <c r="AC45" s="76" t="s">
         <v>18</v>
       </c>
-      <c r="AD45" s="88" t="s">
+      <c r="AD45" s="77" t="s">
         <v>125</v>
       </c>
-      <c r="AE45" s="72" t="s">
-        <v>294</v>
-      </c>
-      <c r="AF45" s="72">
-        <v>1</v>
-      </c>
-      <c r="AG45" s="77" t="s">
+      <c r="AE45" s="64" t="s">
+        <v>294</v>
+      </c>
+      <c r="AF45" s="64">
+        <v>1</v>
+      </c>
+      <c r="AG45" s="68" t="s">
         <v>308</v>
       </c>
-      <c r="AH45" s="72">
+      <c r="AH45" s="64">
         <v>70000</v>
       </c>
-      <c r="AI45" s="65"/>
+      <c r="AI45" s="58"/>
       <c r="AJ45" s="1" t="s">
         <v>266</v>
       </c>
@@ -4986,10 +4977,10 @@
       <c r="AM45" s="1" t="s">
         <v>125</v>
       </c>
-      <c r="AN45" s="73" t="s">
-        <v>294</v>
-      </c>
-      <c r="AO45" s="68">
+      <c r="AN45" s="65" t="s">
+        <v>294</v>
+      </c>
+      <c r="AO45" s="61">
         <v>1</v>
       </c>
       <c r="AP45" s="1">
@@ -5028,31 +5019,31 @@
       <c r="Y46" s="1" t="s">
         <v>306</v>
       </c>
-      <c r="AA46" s="72" t="s">
+      <c r="AA46" s="64" t="s">
         <v>238</v>
       </c>
-      <c r="AB46" s="85" t="s">
+      <c r="AB46" s="74" t="s">
         <v>178</v>
       </c>
-      <c r="AC46" s="87" t="s">
+      <c r="AC46" s="76" t="s">
         <v>18</v>
       </c>
-      <c r="AD46" s="88" t="s">
+      <c r="AD46" s="77" t="s">
         <v>126</v>
       </c>
-      <c r="AE46" s="72" t="s">
-        <v>294</v>
-      </c>
-      <c r="AF46" s="72">
-        <v>1</v>
-      </c>
-      <c r="AG46" s="77" t="s">
+      <c r="AE46" s="64" t="s">
+        <v>294</v>
+      </c>
+      <c r="AF46" s="64">
+        <v>1</v>
+      </c>
+      <c r="AG46" s="68" t="s">
         <v>308</v>
       </c>
-      <c r="AH46" s="72">
+      <c r="AH46" s="64">
         <v>70000</v>
       </c>
-      <c r="AI46" s="65"/>
+      <c r="AI46" s="58"/>
       <c r="AJ46" s="1" t="s">
         <v>267</v>
       </c>
@@ -5065,10 +5056,10 @@
       <c r="AM46" s="1" t="s">
         <v>126</v>
       </c>
-      <c r="AN46" s="73" t="s">
-        <v>294</v>
-      </c>
-      <c r="AO46" s="68">
+      <c r="AN46" s="65" t="s">
+        <v>294</v>
+      </c>
+      <c r="AO46" s="61">
         <v>1</v>
       </c>
       <c r="AP46" s="1">
@@ -5107,31 +5098,31 @@
       <c r="Y47" s="1" t="s">
         <v>306</v>
       </c>
-      <c r="AA47" s="72" t="s">
+      <c r="AA47" s="64" t="s">
         <v>239</v>
       </c>
-      <c r="AB47" s="85" t="s">
+      <c r="AB47" s="74" t="s">
         <v>178</v>
       </c>
-      <c r="AC47" s="87" t="s">
+      <c r="AC47" s="76" t="s">
         <v>18</v>
       </c>
-      <c r="AD47" s="88" t="s">
+      <c r="AD47" s="77" t="s">
         <v>127</v>
       </c>
-      <c r="AE47" s="72" t="s">
-        <v>294</v>
-      </c>
-      <c r="AF47" s="72">
-        <v>1</v>
-      </c>
-      <c r="AG47" s="77" t="s">
+      <c r="AE47" s="64" t="s">
+        <v>294</v>
+      </c>
+      <c r="AF47" s="64">
+        <v>1</v>
+      </c>
+      <c r="AG47" s="68" t="s">
         <v>308</v>
       </c>
-      <c r="AH47" s="72">
+      <c r="AH47" s="64">
         <v>70000</v>
       </c>
-      <c r="AI47" s="65"/>
+      <c r="AI47" s="58"/>
       <c r="AJ47" s="1" t="s">
         <v>268</v>
       </c>
@@ -5144,10 +5135,10 @@
       <c r="AM47" s="1" t="s">
         <v>127</v>
       </c>
-      <c r="AN47" s="73" t="s">
-        <v>294</v>
-      </c>
-      <c r="AO47" s="68">
+      <c r="AN47" s="65" t="s">
+        <v>294</v>
+      </c>
+      <c r="AO47" s="61">
         <v>1</v>
       </c>
       <c r="AP47" s="1">
@@ -5186,31 +5177,31 @@
       <c r="Y48" s="1" t="s">
         <v>306</v>
       </c>
-      <c r="AA48" s="72" t="s">
+      <c r="AA48" s="64" t="s">
         <v>240</v>
       </c>
-      <c r="AB48" s="85" t="s">
+      <c r="AB48" s="74" t="s">
         <v>178</v>
       </c>
-      <c r="AC48" s="87" t="s">
+      <c r="AC48" s="76" t="s">
         <v>19</v>
       </c>
-      <c r="AD48" s="88" t="s">
+      <c r="AD48" s="77" t="s">
         <v>120</v>
       </c>
-      <c r="AE48" s="72" t="s">
-        <v>294</v>
-      </c>
-      <c r="AF48" s="72">
-        <v>1</v>
-      </c>
-      <c r="AG48" s="77" t="s">
+      <c r="AE48" s="64" t="s">
+        <v>294</v>
+      </c>
+      <c r="AF48" s="64">
+        <v>1</v>
+      </c>
+      <c r="AG48" s="68" t="s">
         <v>308</v>
       </c>
-      <c r="AH48" s="72">
+      <c r="AH48" s="64">
         <v>70000</v>
       </c>
-      <c r="AI48" s="65"/>
+      <c r="AI48" s="58"/>
       <c r="AJ48" s="1" t="s">
         <v>269</v>
       </c>
@@ -5223,10 +5214,10 @@
       <c r="AM48" s="1" t="s">
         <v>120</v>
       </c>
-      <c r="AN48" s="73" t="s">
-        <v>294</v>
-      </c>
-      <c r="AO48" s="68">
+      <c r="AN48" s="65" t="s">
+        <v>294</v>
+      </c>
+      <c r="AO48" s="61">
         <v>1</v>
       </c>
       <c r="AP48" s="1">
@@ -5265,31 +5256,31 @@
       <c r="Y49" s="1" t="s">
         <v>306</v>
       </c>
-      <c r="AA49" s="72" t="s">
+      <c r="AA49" s="64" t="s">
         <v>241</v>
       </c>
-      <c r="AB49" s="85" t="s">
+      <c r="AB49" s="74" t="s">
         <v>178</v>
       </c>
-      <c r="AC49" s="87" t="s">
+      <c r="AC49" s="76" t="s">
         <v>19</v>
       </c>
-      <c r="AD49" s="88" t="s">
+      <c r="AD49" s="77" t="s">
         <v>121</v>
       </c>
-      <c r="AE49" s="72" t="s">
-        <v>294</v>
-      </c>
-      <c r="AF49" s="72">
-        <v>1</v>
-      </c>
-      <c r="AG49" s="77" t="s">
+      <c r="AE49" s="64" t="s">
+        <v>294</v>
+      </c>
+      <c r="AF49" s="64">
+        <v>1</v>
+      </c>
+      <c r="AG49" s="68" t="s">
         <v>308</v>
       </c>
-      <c r="AH49" s="72">
+      <c r="AH49" s="64">
         <v>70000</v>
       </c>
-      <c r="AI49" s="65"/>
+      <c r="AI49" s="58"/>
       <c r="AJ49" s="1" t="s">
         <v>270</v>
       </c>
@@ -5302,10 +5293,10 @@
       <c r="AM49" s="1" t="s">
         <v>121</v>
       </c>
-      <c r="AN49" s="73" t="s">
-        <v>294</v>
-      </c>
-      <c r="AO49" s="68">
+      <c r="AN49" s="65" t="s">
+        <v>294</v>
+      </c>
+      <c r="AO49" s="61">
         <v>1</v>
       </c>
       <c r="AP49" s="1">
@@ -5344,31 +5335,31 @@
       <c r="Y50" s="1" t="s">
         <v>306</v>
       </c>
-      <c r="AA50" s="72" t="s">
+      <c r="AA50" s="64" t="s">
         <v>242</v>
       </c>
-      <c r="AB50" s="85" t="s">
+      <c r="AB50" s="74" t="s">
         <v>178</v>
       </c>
-      <c r="AC50" s="87" t="s">
+      <c r="AC50" s="76" t="s">
         <v>19</v>
       </c>
-      <c r="AD50" s="88" t="s">
+      <c r="AD50" s="77" t="s">
         <v>122</v>
       </c>
-      <c r="AE50" s="72" t="s">
-        <v>294</v>
-      </c>
-      <c r="AF50" s="72">
-        <v>1</v>
-      </c>
-      <c r="AG50" s="77" t="s">
+      <c r="AE50" s="64" t="s">
+        <v>294</v>
+      </c>
+      <c r="AF50" s="64">
+        <v>1</v>
+      </c>
+      <c r="AG50" s="68" t="s">
         <v>308</v>
       </c>
-      <c r="AH50" s="72">
+      <c r="AH50" s="64">
         <v>70000</v>
       </c>
-      <c r="AI50" s="65"/>
+      <c r="AI50" s="58"/>
       <c r="AJ50" s="1" t="s">
         <v>271</v>
       </c>
@@ -5381,10 +5372,10 @@
       <c r="AM50" s="1" t="s">
         <v>122</v>
       </c>
-      <c r="AN50" s="73" t="s">
-        <v>294</v>
-      </c>
-      <c r="AO50" s="68">
+      <c r="AN50" s="65" t="s">
+        <v>294</v>
+      </c>
+      <c r="AO50" s="61">
         <v>1</v>
       </c>
       <c r="AP50" s="1">
@@ -5423,31 +5414,31 @@
       <c r="Y51" s="1" t="s">
         <v>306</v>
       </c>
-      <c r="AA51" s="72" t="s">
+      <c r="AA51" s="64" t="s">
         <v>243</v>
       </c>
-      <c r="AB51" s="85" t="s">
+      <c r="AB51" s="74" t="s">
         <v>178</v>
       </c>
-      <c r="AC51" s="87" t="s">
+      <c r="AC51" s="76" t="s">
         <v>19</v>
       </c>
-      <c r="AD51" s="88" t="s">
+      <c r="AD51" s="77" t="s">
         <v>123</v>
       </c>
-      <c r="AE51" s="72" t="s">
-        <v>294</v>
-      </c>
-      <c r="AF51" s="72">
-        <v>1</v>
-      </c>
-      <c r="AG51" s="77" t="s">
+      <c r="AE51" s="64" t="s">
+        <v>294</v>
+      </c>
+      <c r="AF51" s="64">
+        <v>1</v>
+      </c>
+      <c r="AG51" s="68" t="s">
         <v>308</v>
       </c>
-      <c r="AH51" s="72">
+      <c r="AH51" s="64">
         <v>70000</v>
       </c>
-      <c r="AI51" s="65"/>
+      <c r="AI51" s="58"/>
       <c r="AJ51" s="1" t="s">
         <v>272</v>
       </c>
@@ -5460,10 +5451,10 @@
       <c r="AM51" s="1" t="s">
         <v>123</v>
       </c>
-      <c r="AN51" s="73" t="s">
-        <v>294</v>
-      </c>
-      <c r="AO51" s="68">
+      <c r="AN51" s="65" t="s">
+        <v>294</v>
+      </c>
+      <c r="AO51" s="61">
         <v>1</v>
       </c>
       <c r="AP51" s="1">
@@ -5502,31 +5493,31 @@
       <c r="Y52" s="1" t="s">
         <v>306</v>
       </c>
-      <c r="AA52" s="72" t="s">
+      <c r="AA52" s="64" t="s">
         <v>244</v>
       </c>
-      <c r="AB52" s="85" t="s">
+      <c r="AB52" s="74" t="s">
         <v>178</v>
       </c>
-      <c r="AC52" s="87" t="s">
+      <c r="AC52" s="76" t="s">
         <v>19</v>
       </c>
-      <c r="AD52" s="88" t="s">
+      <c r="AD52" s="77" t="s">
         <v>124</v>
       </c>
-      <c r="AE52" s="72" t="s">
-        <v>294</v>
-      </c>
-      <c r="AF52" s="72">
-        <v>1</v>
-      </c>
-      <c r="AG52" s="77" t="s">
+      <c r="AE52" s="64" t="s">
+        <v>294</v>
+      </c>
+      <c r="AF52" s="64">
+        <v>1</v>
+      </c>
+      <c r="AG52" s="68" t="s">
         <v>308</v>
       </c>
-      <c r="AH52" s="72">
+      <c r="AH52" s="64">
         <v>70000</v>
       </c>
-      <c r="AI52" s="65"/>
+      <c r="AI52" s="58"/>
       <c r="AJ52" s="1" t="s">
         <v>273</v>
       </c>
@@ -5539,10 +5530,10 @@
       <c r="AM52" s="1" t="s">
         <v>124</v>
       </c>
-      <c r="AN52" s="73" t="s">
-        <v>294</v>
-      </c>
-      <c r="AO52" s="68">
+      <c r="AN52" s="65" t="s">
+        <v>294</v>
+      </c>
+      <c r="AO52" s="61">
         <v>1</v>
       </c>
       <c r="AP52" s="1">
@@ -5593,19 +5584,19 @@
       <c r="AD53" s="54" t="s">
         <v>70</v>
       </c>
-      <c r="AE53" s="72" t="s">
-        <v>294</v>
-      </c>
-      <c r="AF53" s="72">
-        <v>1</v>
-      </c>
-      <c r="AG53" s="77" t="s">
+      <c r="AE53" s="64" t="s">
+        <v>294</v>
+      </c>
+      <c r="AF53" s="64">
+        <v>1</v>
+      </c>
+      <c r="AG53" s="68" t="s">
         <v>308</v>
       </c>
       <c r="AH53" s="55">
         <v>90000</v>
       </c>
-      <c r="AI53" s="65"/>
+      <c r="AI53" s="58"/>
     </row>
     <row r="54" spans="13:42" x14ac:dyDescent="0.25">
       <c r="M54" s="17" t="s">
@@ -5651,19 +5642,19 @@
       <c r="AD54" s="54" t="s">
         <v>71</v>
       </c>
-      <c r="AE54" s="72" t="s">
-        <v>294</v>
-      </c>
-      <c r="AF54" s="72">
-        <v>1</v>
-      </c>
-      <c r="AG54" s="77" t="s">
+      <c r="AE54" s="64" t="s">
+        <v>294</v>
+      </c>
+      <c r="AF54" s="64">
+        <v>1</v>
+      </c>
+      <c r="AG54" s="68" t="s">
         <v>308</v>
       </c>
       <c r="AH54" s="55">
         <v>90000</v>
       </c>
-      <c r="AI54" s="65"/>
+      <c r="AI54" s="58"/>
     </row>
     <row r="55" spans="13:42" x14ac:dyDescent="0.25">
       <c r="M55" s="17" t="s">
@@ -5703,25 +5694,25 @@
       <c r="AB55" s="55" t="s">
         <v>178</v>
       </c>
-      <c r="AC55" s="64" t="s">
+      <c r="AC55" s="57" t="s">
         <v>14</v>
       </c>
-      <c r="AD55" s="67" t="s">
+      <c r="AD55" s="60" t="s">
         <v>73</v>
       </c>
-      <c r="AE55" s="72" t="s">
-        <v>294</v>
-      </c>
-      <c r="AF55" s="72">
-        <v>1</v>
-      </c>
-      <c r="AG55" s="77" t="s">
+      <c r="AE55" s="64" t="s">
+        <v>294</v>
+      </c>
+      <c r="AF55" s="64">
+        <v>1</v>
+      </c>
+      <c r="AG55" s="68" t="s">
         <v>308</v>
       </c>
       <c r="AH55" s="55">
         <v>90000</v>
       </c>
-      <c r="AI55" s="65"/>
+      <c r="AI55" s="58"/>
     </row>
     <row r="56" spans="13:42" x14ac:dyDescent="0.25">
       <c r="M56" s="17" t="s">
@@ -5767,19 +5758,19 @@
       <c r="AD56" s="54" t="s">
         <v>70</v>
       </c>
-      <c r="AE56" s="72" t="s">
-        <v>294</v>
-      </c>
-      <c r="AF56" s="72">
-        <v>1</v>
-      </c>
-      <c r="AG56" s="77" t="s">
+      <c r="AE56" s="64" t="s">
+        <v>294</v>
+      </c>
+      <c r="AF56" s="64">
+        <v>1</v>
+      </c>
+      <c r="AG56" s="68" t="s">
         <v>308</v>
       </c>
       <c r="AH56" s="55">
         <v>90000</v>
       </c>
-      <c r="AI56" s="65"/>
+      <c r="AI56" s="58"/>
     </row>
     <row r="57" spans="13:42" x14ac:dyDescent="0.25">
       <c r="M57" s="17" t="s">
@@ -5825,19 +5816,19 @@
       <c r="AD57" s="54" t="s">
         <v>71</v>
       </c>
-      <c r="AE57" s="72" t="s">
-        <v>294</v>
-      </c>
-      <c r="AF57" s="72">
-        <v>1</v>
-      </c>
-      <c r="AG57" s="77" t="s">
+      <c r="AE57" s="64" t="s">
+        <v>294</v>
+      </c>
+      <c r="AF57" s="64">
+        <v>1</v>
+      </c>
+      <c r="AG57" s="68" t="s">
         <v>308</v>
       </c>
       <c r="AH57" s="55">
         <v>90000</v>
       </c>
-      <c r="AI57" s="65"/>
+      <c r="AI57" s="58"/>
     </row>
     <row r="58" spans="13:42" x14ac:dyDescent="0.25">
       <c r="M58" s="17" t="s">
@@ -5871,31 +5862,31 @@
       <c r="Y58" s="1" t="s">
         <v>306</v>
       </c>
-      <c r="AA58" s="79" t="s">
+      <c r="AA58" s="70" t="s">
         <v>279</v>
       </c>
-      <c r="AB58" s="80" t="s">
+      <c r="AB58" s="71" t="s">
         <v>178</v>
       </c>
-      <c r="AC58" s="64" t="s">
+      <c r="AC58" s="57" t="s">
         <v>15</v>
       </c>
-      <c r="AD58" s="67" t="s">
+      <c r="AD58" s="60" t="s">
         <v>165</v>
       </c>
-      <c r="AE58" s="72" t="s">
-        <v>294</v>
-      </c>
-      <c r="AF58" s="72">
-        <v>1</v>
-      </c>
-      <c r="AG58" s="77" t="s">
+      <c r="AE58" s="64" t="s">
+        <v>294</v>
+      </c>
+      <c r="AF58" s="64">
+        <v>1</v>
+      </c>
+      <c r="AG58" s="68" t="s">
         <v>308</v>
       </c>
-      <c r="AH58" s="80">
+      <c r="AH58" s="71">
         <v>90000</v>
       </c>
-      <c r="AI58" s="65"/>
+      <c r="AI58" s="58"/>
     </row>
     <row r="59" spans="13:42" x14ac:dyDescent="0.25">
       <c r="M59" s="17" t="s">
@@ -5941,19 +5932,19 @@
       <c r="AD59" s="54" t="s">
         <v>166</v>
       </c>
-      <c r="AE59" s="72" t="s">
-        <v>294</v>
-      </c>
-      <c r="AF59" s="72">
-        <v>1</v>
-      </c>
-      <c r="AG59" s="77" t="s">
+      <c r="AE59" s="64" t="s">
+        <v>294</v>
+      </c>
+      <c r="AF59" s="64">
+        <v>1</v>
+      </c>
+      <c r="AG59" s="68" t="s">
         <v>308</v>
       </c>
       <c r="AH59" s="55">
         <v>90000</v>
       </c>
-      <c r="AI59" s="65"/>
+      <c r="AI59" s="58"/>
     </row>
     <row r="60" spans="13:42" x14ac:dyDescent="0.25">
       <c r="M60" s="17" t="s">
@@ -5999,19 +5990,19 @@
       <c r="AD60" s="54" t="s">
         <v>73</v>
       </c>
-      <c r="AE60" s="72" t="s">
-        <v>294</v>
-      </c>
-      <c r="AF60" s="72">
-        <v>1</v>
-      </c>
-      <c r="AG60" s="77" t="s">
+      <c r="AE60" s="64" t="s">
+        <v>294</v>
+      </c>
+      <c r="AF60" s="64">
+        <v>1</v>
+      </c>
+      <c r="AG60" s="68" t="s">
         <v>308</v>
       </c>
       <c r="AH60" s="55">
         <v>90000</v>
       </c>
-      <c r="AI60" s="65"/>
+      <c r="AI60" s="58"/>
     </row>
     <row r="61" spans="13:42" x14ac:dyDescent="0.25">
       <c r="M61" s="13" t="s">
@@ -6057,19 +6048,19 @@
       <c r="AD61" s="9" t="s">
         <v>143</v>
       </c>
-      <c r="AE61" s="72" t="s">
-        <v>294</v>
-      </c>
-      <c r="AF61" s="72">
-        <v>1</v>
-      </c>
-      <c r="AG61" s="77" t="s">
+      <c r="AE61" s="64" t="s">
+        <v>294</v>
+      </c>
+      <c r="AF61" s="64">
+        <v>1</v>
+      </c>
+      <c r="AG61" s="68" t="s">
         <v>308</v>
       </c>
       <c r="AH61" s="55">
         <v>90000</v>
       </c>
-      <c r="AI61" s="65"/>
+      <c r="AI61" s="58"/>
     </row>
     <row r="62" spans="13:42" ht="15.75" x14ac:dyDescent="0.25">
       <c r="M62" s="13" t="s">
@@ -6115,19 +6106,19 @@
       <c r="AD62" s="9" t="s">
         <v>144</v>
       </c>
-      <c r="AE62" s="72" t="s">
-        <v>294</v>
-      </c>
-      <c r="AF62" s="72">
-        <v>1</v>
-      </c>
-      <c r="AG62" s="77" t="s">
+      <c r="AE62" s="64" t="s">
+        <v>294</v>
+      </c>
+      <c r="AF62" s="64">
+        <v>1</v>
+      </c>
+      <c r="AG62" s="68" t="s">
         <v>308</v>
       </c>
       <c r="AH62" s="55">
         <v>90000</v>
       </c>
-      <c r="AI62" s="65"/>
+      <c r="AI62" s="58"/>
     </row>
     <row r="63" spans="13:42" ht="15.75" x14ac:dyDescent="0.25">
       <c r="M63" s="13" t="s">
@@ -6161,15 +6152,15 @@
       <c r="Y63" s="10" t="s">
         <v>305</v>
       </c>
-      <c r="AA63" s="65"/>
-      <c r="AB63" s="65"/>
-      <c r="AC63" s="66"/>
-      <c r="AD63" s="67"/>
-      <c r="AE63" s="65"/>
-      <c r="AF63" s="65"/>
-      <c r="AG63" s="65"/>
-      <c r="AH63" s="65"/>
-      <c r="AI63" s="65"/>
+      <c r="AA63" s="58"/>
+      <c r="AB63" s="58"/>
+      <c r="AC63" s="59"/>
+      <c r="AD63" s="60"/>
+      <c r="AE63" s="58"/>
+      <c r="AF63" s="58"/>
+      <c r="AG63" s="58"/>
+      <c r="AH63" s="58"/>
+      <c r="AI63" s="58"/>
     </row>
     <row r="64" spans="13:42" ht="15.75" x14ac:dyDescent="0.25">
       <c r="M64" s="13" t="s">
@@ -6203,15 +6194,15 @@
       <c r="Y64" s="10" t="s">
         <v>305</v>
       </c>
-      <c r="AA64" s="65"/>
-      <c r="AB64" s="65"/>
-      <c r="AC64" s="66"/>
-      <c r="AD64" s="67"/>
-      <c r="AE64" s="65"/>
-      <c r="AF64" s="65"/>
-      <c r="AG64" s="65"/>
-      <c r="AH64" s="65"/>
-      <c r="AI64" s="65"/>
+      <c r="AA64" s="58"/>
+      <c r="AB64" s="58"/>
+      <c r="AC64" s="59"/>
+      <c r="AD64" s="60"/>
+      <c r="AE64" s="58"/>
+      <c r="AF64" s="58"/>
+      <c r="AG64" s="58"/>
+      <c r="AH64" s="58"/>
+      <c r="AI64" s="58"/>
     </row>
     <row r="65" spans="13:35" ht="15.75" x14ac:dyDescent="0.25">
       <c r="M65" s="13" t="s">
@@ -6245,15 +6236,15 @@
       <c r="Y65" s="10" t="s">
         <v>305</v>
       </c>
-      <c r="AA65" s="65"/>
-      <c r="AB65" s="65"/>
-      <c r="AC65" s="66"/>
-      <c r="AD65" s="67"/>
-      <c r="AE65" s="65"/>
-      <c r="AF65" s="65"/>
-      <c r="AG65" s="65"/>
-      <c r="AH65" s="65"/>
-      <c r="AI65" s="65"/>
+      <c r="AA65" s="58"/>
+      <c r="AB65" s="58"/>
+      <c r="AC65" s="59"/>
+      <c r="AD65" s="60"/>
+      <c r="AE65" s="58"/>
+      <c r="AF65" s="58"/>
+      <c r="AG65" s="58"/>
+      <c r="AH65" s="58"/>
+      <c r="AI65" s="58"/>
     </row>
     <row r="66" spans="13:35" ht="15.75" x14ac:dyDescent="0.25">
       <c r="M66" s="31" t="s">
@@ -6287,15 +6278,15 @@
       <c r="Y66" s="10" t="s">
         <v>305</v>
       </c>
-      <c r="AA66" s="65"/>
-      <c r="AB66" s="65"/>
-      <c r="AC66" s="66"/>
-      <c r="AD66" s="67"/>
-      <c r="AE66" s="65"/>
-      <c r="AF66" s="65"/>
-      <c r="AG66" s="65"/>
-      <c r="AH66" s="65"/>
-      <c r="AI66" s="65"/>
+      <c r="AA66" s="58"/>
+      <c r="AB66" s="58"/>
+      <c r="AC66" s="59"/>
+      <c r="AD66" s="60"/>
+      <c r="AE66" s="58"/>
+      <c r="AF66" s="58"/>
+      <c r="AG66" s="58"/>
+      <c r="AH66" s="58"/>
+      <c r="AI66" s="58"/>
     </row>
     <row r="67" spans="13:35" ht="15.75" x14ac:dyDescent="0.25">
       <c r="M67" s="31" t="s">
@@ -6329,15 +6320,15 @@
       <c r="Y67" s="10" t="s">
         <v>305</v>
       </c>
-      <c r="AA67" s="65"/>
-      <c r="AB67" s="65"/>
-      <c r="AC67" s="66"/>
-      <c r="AD67" s="67"/>
-      <c r="AE67" s="65"/>
-      <c r="AF67" s="65"/>
-      <c r="AG67" s="65"/>
-      <c r="AH67" s="65"/>
-      <c r="AI67" s="65"/>
+      <c r="AA67" s="58"/>
+      <c r="AB67" s="58"/>
+      <c r="AC67" s="59"/>
+      <c r="AD67" s="60"/>
+      <c r="AE67" s="58"/>
+      <c r="AF67" s="58"/>
+      <c r="AG67" s="58"/>
+      <c r="AH67" s="58"/>
+      <c r="AI67" s="58"/>
     </row>
     <row r="68" spans="13:35" ht="15.75" x14ac:dyDescent="0.25">
       <c r="M68" s="31" t="s">
@@ -6371,98 +6362,84 @@
       <c r="Y68" s="10" t="s">
         <v>305</v>
       </c>
-      <c r="AA68" s="65"/>
-      <c r="AB68" s="65"/>
-      <c r="AC68" s="66"/>
-      <c r="AD68" s="67"/>
-      <c r="AE68" s="65"/>
-      <c r="AF68" s="65"/>
-      <c r="AG68" s="65"/>
-      <c r="AH68" s="65"/>
-      <c r="AI68" s="65"/>
+      <c r="AA68" s="58"/>
+      <c r="AB68" s="58"/>
+      <c r="AC68" s="59"/>
+      <c r="AD68" s="60"/>
+      <c r="AE68" s="58"/>
+      <c r="AF68" s="58"/>
+      <c r="AG68" s="58"/>
+      <c r="AH68" s="58"/>
+      <c r="AI68" s="58"/>
     </row>
     <row r="69" spans="13:35" x14ac:dyDescent="0.25">
-      <c r="AA69" s="65"/>
-      <c r="AB69" s="65"/>
-      <c r="AC69" s="66"/>
-      <c r="AD69" s="67"/>
-      <c r="AE69" s="65"/>
-      <c r="AF69" s="65"/>
-      <c r="AG69" s="65"/>
-      <c r="AH69" s="65"/>
-      <c r="AI69" s="65"/>
+      <c r="AA69" s="58"/>
+      <c r="AB69" s="58"/>
+      <c r="AC69" s="59"/>
+      <c r="AD69" s="60"/>
+      <c r="AE69" s="58"/>
+      <c r="AF69" s="58"/>
+      <c r="AG69" s="58"/>
+      <c r="AH69" s="58"/>
+      <c r="AI69" s="58"/>
     </row>
     <row r="70" spans="13:35" x14ac:dyDescent="0.25">
-      <c r="AA70" s="65"/>
-      <c r="AB70" s="65"/>
-      <c r="AC70" s="66"/>
-      <c r="AD70" s="67"/>
-      <c r="AE70" s="65"/>
-      <c r="AF70" s="65"/>
-      <c r="AG70" s="65"/>
-      <c r="AH70" s="65"/>
-      <c r="AI70" s="65"/>
+      <c r="AA70" s="58"/>
+      <c r="AB70" s="58"/>
+      <c r="AC70" s="59"/>
+      <c r="AD70" s="60"/>
+      <c r="AE70" s="58"/>
+      <c r="AF70" s="58"/>
+      <c r="AG70" s="58"/>
+      <c r="AH70" s="58"/>
+      <c r="AI70" s="58"/>
     </row>
     <row r="71" spans="13:35" x14ac:dyDescent="0.25">
-      <c r="AA71" s="65"/>
-      <c r="AB71" s="65"/>
-      <c r="AC71" s="66"/>
-      <c r="AD71" s="67"/>
-      <c r="AE71" s="65"/>
-      <c r="AF71" s="65"/>
-      <c r="AG71" s="65"/>
-      <c r="AH71" s="65"/>
-      <c r="AI71" s="65"/>
+      <c r="AA71" s="58"/>
+      <c r="AB71" s="58"/>
+      <c r="AC71" s="59"/>
+      <c r="AD71" s="60"/>
+      <c r="AE71" s="58"/>
+      <c r="AF71" s="58"/>
+      <c r="AG71" s="58"/>
+      <c r="AH71" s="58"/>
+      <c r="AI71" s="58"/>
     </row>
     <row r="72" spans="13:35" x14ac:dyDescent="0.25">
-      <c r="AA72" s="65"/>
-      <c r="AB72" s="65"/>
-      <c r="AC72" s="66"/>
-      <c r="AD72" s="67"/>
-      <c r="AE72" s="65"/>
-      <c r="AF72" s="65"/>
-      <c r="AG72" s="65"/>
-      <c r="AH72" s="65"/>
-      <c r="AI72" s="65"/>
+      <c r="AA72" s="58"/>
+      <c r="AB72" s="58"/>
+      <c r="AC72" s="59"/>
+      <c r="AD72" s="60"/>
+      <c r="AE72" s="58"/>
+      <c r="AF72" s="58"/>
+      <c r="AG72" s="58"/>
+      <c r="AH72" s="58"/>
+      <c r="AI72" s="58"/>
     </row>
     <row r="73" spans="13:35" x14ac:dyDescent="0.25">
-      <c r="AA73" s="65"/>
-      <c r="AB73" s="65"/>
-      <c r="AC73" s="66"/>
-      <c r="AD73" s="67"/>
-      <c r="AE73" s="65"/>
-      <c r="AF73" s="65"/>
-      <c r="AG73" s="65"/>
-      <c r="AH73" s="65"/>
-      <c r="AI73" s="65"/>
+      <c r="AA73" s="58"/>
+      <c r="AB73" s="58"/>
+      <c r="AC73" s="59"/>
+      <c r="AD73" s="60"/>
+      <c r="AE73" s="58"/>
+      <c r="AF73" s="58"/>
+      <c r="AG73" s="58"/>
+      <c r="AH73" s="58"/>
+      <c r="AI73" s="58"/>
     </row>
     <row r="74" spans="13:35" x14ac:dyDescent="0.25">
-      <c r="AA74" s="65"/>
-      <c r="AB74" s="65"/>
-      <c r="AC74" s="66"/>
-      <c r="AD74" s="67"/>
-      <c r="AE74" s="65"/>
-      <c r="AF74" s="65"/>
-      <c r="AG74" s="65"/>
-      <c r="AH74" s="65"/>
-      <c r="AI74" s="65"/>
+      <c r="AA74" s="58"/>
+      <c r="AB74" s="58"/>
+      <c r="AC74" s="59"/>
+      <c r="AD74" s="60"/>
+      <c r="AE74" s="58"/>
+      <c r="AF74" s="58"/>
+      <c r="AG74" s="58"/>
+      <c r="AH74" s="58"/>
+      <c r="AI74" s="58"/>
     </row>
   </sheetData>
   <mergeCells count="30">
-    <mergeCell ref="P21:R21"/>
-    <mergeCell ref="P22:R22"/>
-    <mergeCell ref="P23:R23"/>
-    <mergeCell ref="P16:R16"/>
-    <mergeCell ref="P17:R17"/>
-    <mergeCell ref="P18:R18"/>
-    <mergeCell ref="P19:R19"/>
-    <mergeCell ref="P20:R20"/>
-    <mergeCell ref="AA14:AH14"/>
-    <mergeCell ref="AJ14:AP14"/>
-    <mergeCell ref="AN2:AO2"/>
-    <mergeCell ref="C2:F2"/>
-    <mergeCell ref="S2:T2"/>
-    <mergeCell ref="C14:H14"/>
     <mergeCell ref="B15:K15"/>
     <mergeCell ref="M14:Y14"/>
     <mergeCell ref="P15:R15"/>
@@ -6479,6 +6456,20 @@
     <mergeCell ref="AA2:AJ2"/>
     <mergeCell ref="AB12:AI12"/>
     <mergeCell ref="V2:W2"/>
+    <mergeCell ref="AA14:AH14"/>
+    <mergeCell ref="AJ14:AP14"/>
+    <mergeCell ref="AN2:AO2"/>
+    <mergeCell ref="C2:F2"/>
+    <mergeCell ref="S2:T2"/>
+    <mergeCell ref="C14:H14"/>
+    <mergeCell ref="P21:R21"/>
+    <mergeCell ref="P22:R22"/>
+    <mergeCell ref="P23:R23"/>
+    <mergeCell ref="P16:R16"/>
+    <mergeCell ref="P17:R17"/>
+    <mergeCell ref="P18:R18"/>
+    <mergeCell ref="P19:R19"/>
+    <mergeCell ref="P20:R20"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>

</xml_diff>